<commit_message>
Portfolio and risk week 3.
</commit_message>
<xml_diff>
--- a/ClassesTaken/Coursera/2016/InvManagementRice/02PortfolioRisk/PortfolioRisk.xlsx
+++ b/ClassesTaken/Coursera/2016/InvManagementRice/02PortfolioRisk/PortfolioRisk.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14928" windowHeight="8076" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14928" windowHeight="8076" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="wk01" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="covHw3_2" sheetId="5" r:id="rId5"/>
     <sheet name="covHw3data" sheetId="6" r:id="rId6"/>
     <sheet name="Hw3chart" sheetId="7" r:id="rId7"/>
+    <sheet name="wk03" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="139">
   <si>
     <t>P0</t>
   </si>
@@ -431,6 +432,39 @@
   <si>
     <t>Invested</t>
   </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Treasuries</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
 </sst>
 </file>
 
@@ -527,7 +561,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
@@ -562,6 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -569,9 +604,153 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="296">
-    <dxf>
+  <dxfs count="313">
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -593,6 +772,9 @@
       <numFmt numFmtId="168" formatCode="0.00000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -612,6 +794,9 @@
       <numFmt numFmtId="168" formatCode="0.00000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -631,6 +816,9 @@
       <numFmt numFmtId="169" formatCode="0.000000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="169" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -650,6 +838,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -669,6 +860,9 @@
       <numFmt numFmtId="166" formatCode="0.000%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -688,6 +882,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -707,6 +904,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -726,6 +926,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -745,6 +948,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -818,7 +1024,45 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="167" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="0.0000%"/>
     </dxf>
     <dxf>
       <font>
@@ -840,6 +1084,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -932,87 +1179,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="0.0000%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="0.0000%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="0.0000%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000%"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
@@ -1038,6 +1204,9 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1060,10 +1229,23 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <font>
@@ -4145,7 +4327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FFFDFA2-A312-4FA2-B67A-4860469C95AC}" type="CELLRANGE">
+                    <a:fld id="{3D5A4820-3F05-4964-9C96-B0972BAD64B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4178,7 +4360,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{928236D6-89CA-406C-BB7D-F23F0FA969CE}" type="CELLRANGE">
+                    <a:fld id="{2EF7C3E9-5C0B-4DFD-A95F-46B9E41C33A0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4196,7 +4378,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4211,7 +4392,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64B00D5F-6832-4B75-B934-C91867142056}" type="CELLRANGE">
+                    <a:fld id="{8C59BC26-9D00-43EA-87EB-742CD8CB0D41}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4229,7 +4410,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4244,7 +4424,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{317BFBDE-AE66-4725-8B2E-ECF8B15ED3E6}" type="CELLRANGE">
+                    <a:fld id="{49928F6F-AF45-48CF-8BB0-6624BB8B3B6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4262,7 +4442,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4277,7 +4456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89CACBF1-D140-4E75-8DF0-7B6B7EABCFD3}" type="CELLRANGE">
+                    <a:fld id="{C0948C18-DD95-4EFC-838A-47C97C8F07C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4295,7 +4474,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4310,7 +4488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4CF021D-3259-4F48-B95A-AD08642132C6}" type="CELLRANGE">
+                    <a:fld id="{0A022E7B-DFF9-41E4-BE15-F12E2C1AB623}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4328,7 +4506,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4343,7 +4520,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{124F136E-B0E7-4DCE-A308-5D20E4A197D4}" type="CELLRANGE">
+                    <a:fld id="{8F7FABB3-FFB1-4067-9252-96B49D7E670C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4361,7 +4538,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4376,7 +4552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8CCEEB41-B048-40E7-8863-C91C9937F271}" type="CELLRANGE">
+                    <a:fld id="{D948FB4B-10E1-4E7C-B61A-C6CB4BD13FA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4394,7 +4570,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4409,7 +4584,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09043AED-EA70-4413-8E61-B68D2D0163A6}" type="CELLRANGE">
+                    <a:fld id="{2054C994-9C41-434E-B854-1E05ED7A407E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4427,7 +4602,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4442,7 +4616,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4EB54AF3-5586-42A0-8AEA-9999E465C9A8}" type="CELLRANGE">
+                    <a:fld id="{29A048BF-8A5E-46F1-923C-198055E499DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4460,7 +4634,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4475,7 +4648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0011396C-6CDE-4706-9C14-800D126E564F}" type="CELLRANGE">
+                    <a:fld id="{5A9162AA-445A-4636-B759-D5D21CC699AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4493,7 +4666,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4508,7 +4680,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E90E073E-4FB9-4B7F-8831-D23ECCAB809E}" type="CELLRANGE">
+                    <a:fld id="{C566B814-0FB4-48CE-AB65-33165D78FCF1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4526,7 +4698,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4541,7 +4712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD58672B-A5D5-423D-B305-2800E1A0CEE4}" type="CELLRANGE">
+                    <a:fld id="{DB123880-EEA9-4A57-BF73-71769560F4E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4559,7 +4730,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4574,7 +4744,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49C378B2-5472-44D2-B6DF-6D4903DE48DD}" type="CELLRANGE">
+                    <a:fld id="{EBDA353E-6AF4-45EC-B4EB-93B64024D538}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4592,7 +4762,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4607,7 +4776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D59D471-341A-4FBF-BE24-C9AD1E45633B}" type="CELLRANGE">
+                    <a:fld id="{82019887-4446-4352-B922-315327FBA133}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4625,7 +4794,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4640,7 +4808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A3D6E1E-0FC6-4DC4-86EF-66D419A38D5C}" type="CELLRANGE">
+                    <a:fld id="{93EFA4E3-F765-45F6-8AEB-665908864B2D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4658,7 +4826,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4673,7 +4840,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{406B6C4B-AF90-4CAC-8ACF-8C12612CE643}" type="CELLRANGE">
+                    <a:fld id="{9840E6BB-4E9C-47A3-BEA9-0F81B3240122}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4691,7 +4858,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4706,7 +4872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9439FDF1-45BD-4228-9919-3032B488DA1A}" type="CELLRANGE">
+                    <a:fld id="{864F5460-87AA-4BB5-B2D2-F707B3C3D1BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4724,7 +4890,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4739,7 +4904,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4A93EFF-9E1D-48D8-83BC-E5240351A2CE}" type="CELLRANGE">
+                    <a:fld id="{266F8357-D943-43AA-84D9-B15370FF64B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4757,7 +4922,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4772,7 +4936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3F2E64D-DA6D-4B35-B588-D1E403192CD3}" type="CELLRANGE">
+                    <a:fld id="{BF3DF3BC-D7E3-4B51-AB3C-24B3CA5B957F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4790,7 +4954,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4805,7 +4968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ACC63425-135E-4162-8850-D973ED24B06C}" type="CELLRANGE">
+                    <a:fld id="{91EB5A47-469A-4E59-9839-15A0FF14440B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4823,7 +4986,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4838,7 +5000,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82D14F3E-B6C9-4791-A8FC-D4A7B0A73232}" type="CELLRANGE">
+                    <a:fld id="{58F8B8D5-1F8C-4786-8D9D-4B45F0E0A7B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4856,7 +5018,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4871,7 +5032,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9643851-347C-47A9-BBD3-1CF2C3E60A7A}" type="CELLRANGE">
+                    <a:fld id="{4B910AE8-7E10-47F8-9AA9-10A3E5F43E24}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4889,7 +5050,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4904,7 +5064,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE662165-F862-49F6-9F8F-9EC7FCF1ABB2}" type="CELLRANGE">
+                    <a:fld id="{D0229948-1863-4788-8636-2FA751759F93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4922,7 +5082,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4937,7 +5096,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{127AA80D-29FF-46DB-A2DD-361CA4D1B243}" type="CELLRANGE">
+                    <a:fld id="{E204CC38-1EBD-43D4-A42E-93BA5332F365}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4955,7 +5114,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4970,7 +5128,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66F7AFF4-2020-4B7C-8674-CBD1A0B36D92}" type="CELLRANGE">
+                    <a:fld id="{1F1F4B1B-748C-4744-B76D-A3EE34C8664E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4988,7 +5146,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5003,7 +5160,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE8E087D-A13F-49C4-95BE-FE6EE1E0AFCC}" type="CELLRANGE">
+                    <a:fld id="{9C421093-8381-4A02-9C03-710204B3ABD0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5021,7 +5178,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5036,7 +5192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A057D9D-6B61-41AE-9245-8B4B0657A04B}" type="CELLRANGE">
+                    <a:fld id="{B1EF76E3-AA06-490E-83B1-9CE6266E5F92}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5054,7 +5210,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5069,7 +5224,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B25511E-02DB-4EDB-8C40-CD97D3B67902}" type="CELLRANGE">
+                    <a:fld id="{ECF717A1-558B-4308-BBC3-8E49459DC25E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5087,7 +5242,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5102,7 +5256,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBDC8C17-201D-49D9-9335-044CA0DF3869}" type="CELLRANGE">
+                    <a:fld id="{C48E8CA6-9179-488E-BA0C-431DDC68010E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5120,7 +5274,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5135,7 +5288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9A5C32B-7DFB-410C-93CD-5B0E831383C3}" type="CELLRANGE">
+                    <a:fld id="{7697E68E-B9E0-4B1A-856B-DC27D572B609}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5153,7 +5306,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5168,7 +5320,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A0D9C75-3E3A-465D-8533-7DB876679916}" type="CELLRANGE">
+                    <a:fld id="{E1081374-AB01-4655-896D-8F52EAC413E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5186,7 +5338,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5201,7 +5352,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14ECE9E5-C7BF-4E07-800A-689EEF3F1DC4}" type="CELLRANGE">
+                    <a:fld id="{2569A406-9D96-4163-9D7D-FFBB3A45E5B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5219,7 +5370,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5234,7 +5384,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69202E1A-EE26-4327-B6EB-D26856696454}" type="CELLRANGE">
+                    <a:fld id="{26CDA9DF-6167-4F27-9C24-1937736D76DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5252,7 +5402,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5267,7 +5416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFC2621A-7F1C-4EED-A6FE-9D22C558D35B}" type="CELLRANGE">
+                    <a:fld id="{A61BA4FB-215D-4593-A67F-6BC82F1F8ADD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5285,7 +5434,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5300,7 +5448,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B2B2D67-B7AC-4A20-BF93-CBA62CA86B23}" type="CELLRANGE">
+                    <a:fld id="{9F75F754-F24A-4843-8E6D-0F2A0EC60209}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5318,7 +5466,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5333,7 +5480,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA1A3B74-6FC6-460E-B8F5-B98BDB066521}" type="CELLRANGE">
+                    <a:fld id="{2C6381FC-5733-4BA5-AF44-D38AD93E4F8B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5351,7 +5498,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5366,7 +5512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B32A7E80-F144-4B24-BFE3-3147D938D0F8}" type="CELLRANGE">
+                    <a:fld id="{0C9FEF8E-8838-410C-822D-10F5F230388B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5384,7 +5530,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5399,7 +5544,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{841C7D16-0847-4F32-A932-77B177E782BC}" type="CELLRANGE">
+                    <a:fld id="{E1467B2F-19D7-4E2A-930B-4B7C3A40DFCF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5417,7 +5562,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5432,7 +5576,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDAE92BB-2A24-4CBA-90EF-307D8D9C03D4}" type="CELLRANGE">
+                    <a:fld id="{51DA1B63-8AA8-44EA-B63C-895D6761BACB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5450,7 +5594,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5465,7 +5608,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67A71237-6D4E-44C1-8259-E7D90994BC30}" type="CELLRANGE">
+                    <a:fld id="{F058E486-CECC-40F2-8D83-346DE3DF0AF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5483,7 +5626,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5498,7 +5640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C3EBA45-DF42-4D3C-82CE-665A8B5E2878}" type="CELLRANGE">
+                    <a:fld id="{3D00FC07-7365-4853-A951-BEA3E49430DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5516,7 +5658,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5531,7 +5672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CED2024-A7D4-4098-B3FC-547A85369D45}" type="CELLRANGE">
+                    <a:fld id="{41919063-E0E6-4D09-AABD-51C60858ABD1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5549,7 +5690,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5564,7 +5704,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{625BB321-67E7-4D8F-AD36-BA125D82C678}" type="CELLRANGE">
+                    <a:fld id="{495AEF83-887D-4441-BAFF-9A3470FC3796}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5582,7 +5722,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5597,7 +5736,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B962C5E6-50EA-4704-B0C5-C12F49F5B8F3}" type="CELLRANGE">
+                    <a:fld id="{C7CF26D3-DCE9-4480-9A35-B483E60B414A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5615,7 +5754,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5630,7 +5768,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EECEC45-8ACB-42D1-AA55-826FB9F10300}" type="CELLRANGE">
+                    <a:fld id="{55610D42-5CC7-4069-976A-309AA281BE67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5648,7 +5786,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5663,7 +5800,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D8C0414-A2DE-4524-898B-CBF7951BA102}" type="CELLRANGE">
+                    <a:fld id="{3C0AB8FB-1566-46FC-B4E6-D85B0F39F82F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5681,7 +5818,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5696,7 +5832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC574A07-2B3C-4CFF-9866-4476FA44ECEA}" type="CELLRANGE">
+                    <a:fld id="{21B414A3-CEFE-41F0-B781-CB6EBC37602B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5714,7 +5850,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5729,7 +5864,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A22765F-A030-4399-8C26-806A8DE53854}" type="CELLRANGE">
+                    <a:fld id="{56305D20-94EF-4F2F-A0A7-A399CCF6199B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5747,7 +5882,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5762,7 +5896,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59F3BCB8-E9BE-4873-A47E-3FC5DEC7D091}" type="CELLRANGE">
+                    <a:fld id="{6067DE17-C64B-4FA9-BF47-6FC244B5E0AA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5780,7 +5914,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5795,7 +5928,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B05B77B-BD00-4A73-A9CF-FF6894EDE7CC}" type="CELLRANGE">
+                    <a:fld id="{9CC69B2D-59BB-496C-8837-96FE3FA7A0BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5828,7 +5961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31611A8A-127D-4683-AF60-0BE43FBAE9EC}" type="CELLRANGE">
+                    <a:fld id="{DA1D1933-8255-4587-828F-DAE0CD56072B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5846,7 +5979,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5861,7 +5993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9ED92329-22C6-41EB-9757-A82975332B8C}" type="CELLRANGE">
+                    <a:fld id="{4468F7A5-D9C2-44A9-A288-76FD6A9EA9D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5879,7 +6011,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5894,7 +6025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D659FEA-C2C6-4B69-88C5-B07BEC707627}" type="CELLRANGE">
+                    <a:fld id="{F64091AF-1066-405A-B720-206CA90307A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5912,7 +6043,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5927,7 +6057,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{807566EB-17D1-4728-82CF-0488E661CBC4}" type="CELLRANGE">
+                    <a:fld id="{22D97079-61EB-41CA-9C10-530E6C3C065A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5945,7 +6075,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5960,7 +6089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68C4CDDC-AA97-4EAC-9C9F-22479F2AEE18}" type="CELLRANGE">
+                    <a:fld id="{34E2345B-B469-4377-B04B-B3F8D8060B99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5978,7 +6107,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5993,7 +6121,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFF88C7D-F841-4EAE-89B2-929B13533FB5}" type="CELLRANGE">
+                    <a:fld id="{ABB5E11F-C6D5-4E6C-BB81-F345DB8964AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6011,7 +6139,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6026,7 +6153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F572A64F-DFDD-44DD-B0F9-5015AEAAF883}" type="CELLRANGE">
+                    <a:fld id="{1FB38142-9A1F-4E7B-8D18-8578FFDDA748}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6044,7 +6171,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6059,7 +6185,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA1635A4-6C34-49FB-A29D-A2BF27AB195E}" type="CELLRANGE">
+                    <a:fld id="{D5D9CB81-EE10-4FEB-84BC-8262E68B875E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6077,7 +6203,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6092,7 +6217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{652518C3-AAE3-4456-9CB8-F8A8CD81BA7D}" type="CELLRANGE">
+                    <a:fld id="{C5C24F7E-A335-48A6-B4CD-1A2231B8D84B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6110,7 +6235,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6125,7 +6249,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{088E7CE9-6DE8-4D21-8613-8F90A1CB07DE}" type="CELLRANGE">
+                    <a:fld id="{17B44E5D-5BEF-4DB9-A678-AAE2EED31641}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6143,7 +6267,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6158,7 +6281,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D8CFD74-07BA-4E1F-A244-94C0B82B2211}" type="CELLRANGE">
+                    <a:fld id="{EDBC9B43-421C-4C1A-82A0-2EC57000B919}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6176,7 +6299,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6191,7 +6313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A17F46A-21AA-4B63-81DA-3F820E264F64}" type="CELLRANGE">
+                    <a:fld id="{351BF981-2A76-4BFB-89DB-1970B94F27B6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6209,7 +6331,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6224,7 +6345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28EEA0DD-7B12-4632-B970-28A5200ED1CD}" type="CELLRANGE">
+                    <a:fld id="{8DABD37D-4DEC-40C8-A966-8E11C26E97D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6242,7 +6363,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6257,7 +6377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{720B64BC-030E-446E-84EB-FAC86A2FDD49}" type="CELLRANGE">
+                    <a:fld id="{19C9FA57-E595-4606-8A6D-5FC6C50262BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6275,7 +6395,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6290,7 +6409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77088DFC-4BA2-4883-8B5B-C6FAF7F4EE1E}" type="CELLRANGE">
+                    <a:fld id="{EC035C02-650E-4733-B144-90FB15DBD353}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6308,7 +6427,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6323,7 +6441,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7683254B-354F-44EC-99DF-8B426771A37B}" type="CELLRANGE">
+                    <a:fld id="{F3A41DDB-3C1C-49F2-AC32-F409CB48A81C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6341,7 +6459,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6356,7 +6473,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A44B13CA-FA00-4ABB-B6BA-BD238250BA02}" type="CELLRANGE">
+                    <a:fld id="{160A819D-0064-411E-B95A-366D0F21C5BD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6374,7 +6491,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6389,7 +6505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9268C71-E6F8-4CA7-8059-CEF5B280E711}" type="CELLRANGE">
+                    <a:fld id="{25934EE9-18FF-4D91-8595-45849EB98525}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6407,7 +6523,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6422,7 +6537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5DED4A05-3C5D-4D3B-9FD2-EAE9C44632B6}" type="CELLRANGE">
+                    <a:fld id="{2B7B8B5E-614F-47F0-84D7-62371EE9AA9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6440,7 +6555,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6455,7 +6569,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AC14ABC-3CAE-467B-A862-63FA3C6455AC}" type="CELLRANGE">
+                    <a:fld id="{A0F029D3-F6F7-4ABC-860D-6D6709803C80}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6473,7 +6587,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6488,7 +6601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFBB3B11-BC8D-421D-A683-D7301387C1CF}" type="CELLRANGE">
+                    <a:fld id="{397BB740-7000-46AF-AB9C-F4A3A2CCF2FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6506,7 +6619,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6521,7 +6633,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00E24A10-8A68-4D37-8A49-7EA37A44ED19}" type="CELLRANGE">
+                    <a:fld id="{821248B2-3E06-46E0-98F2-778385FA03B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6539,7 +6651,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6554,7 +6665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{645F2437-16E7-4E08-AE86-0AB50EFFAAE1}" type="CELLRANGE">
+                    <a:fld id="{1A203DE8-A5E3-4ADA-A99D-1B3AA2848B02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6572,7 +6683,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6587,7 +6697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6043169-CF36-41ED-BF72-4913EFFD5C88}" type="CELLRANGE">
+                    <a:fld id="{7202B26D-3070-4B86-8F33-1F2CC1BD2F48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6605,7 +6715,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6620,7 +6729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{10143AFF-E0A2-431D-B336-8DBF40ED65E8}" type="CELLRANGE">
+                    <a:fld id="{2AEC927C-6952-4D3E-822C-931218B99934}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6638,7 +6747,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6653,7 +6761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0C9DD0C-AB7E-4D8E-89D8-8A2F5AD2CE3E}" type="CELLRANGE">
+                    <a:fld id="{04CE457D-E011-480F-911D-514D3190E39F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6671,7 +6779,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6686,7 +6793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05C1B023-0842-4248-93C9-7A119E87E989}" type="CELLRANGE">
+                    <a:fld id="{4964FC94-B544-4934-9D01-AF12B495EC4F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6704,7 +6811,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6719,7 +6825,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38AB5E51-3ACA-4005-8A81-CC1515BE5345}" type="CELLRANGE">
+                    <a:fld id="{27222FFE-AA8E-4345-A456-F0FA83DFCDB2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6737,7 +6843,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6752,7 +6857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56DC3731-743A-4445-97D3-7D8D81F67787}" type="CELLRANGE">
+                    <a:fld id="{1ABAD332-269B-4F4C-A332-F86E20A6A883}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6770,7 +6875,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6785,7 +6889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{545B875C-D3B7-49A8-A621-BA512C98612F}" type="CELLRANGE">
+                    <a:fld id="{3E59BE2D-0DFE-4DD9-A3BB-C23ED465E001}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6803,7 +6907,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6818,7 +6921,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89D0AD23-D411-4E68-AACA-D3CB4D09FEDC}" type="CELLRANGE">
+                    <a:fld id="{CC5E4F2D-B3E4-4B27-8033-2B95E3C9116A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6836,7 +6939,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6851,7 +6953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D59DDFEB-24A2-4E97-A9C2-31EA0CE41273}" type="CELLRANGE">
+                    <a:fld id="{6B72154C-5745-4E4A-9285-5B2F09F5D830}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6869,7 +6971,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6884,7 +6985,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8ECDA571-3C95-425F-8013-440DA26E9221}" type="CELLRANGE">
+                    <a:fld id="{797DD8E5-FE59-4BCB-85EF-868F1D50F57D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6902,7 +7003,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6917,7 +7017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB8B9B65-B640-48BF-BB0E-1F458E8FA86D}" type="CELLRANGE">
+                    <a:fld id="{0048AB6B-7E45-4BCF-881E-5E0C8FE1CE6A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6935,7 +7035,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6950,7 +7049,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E578DE4-6967-40B8-A5D6-1775CA004CAE}" type="CELLRANGE">
+                    <a:fld id="{85CC1774-FDBD-46DA-81E2-0B4BE25EEFE4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6968,7 +7067,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6983,7 +7081,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2E2C9B1-E8AC-4EBC-AB51-2FD538F52530}" type="CELLRANGE">
+                    <a:fld id="{2F64B4BD-E220-41F4-8BE2-7485D7F164A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7001,7 +7099,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7016,7 +7113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D67BB58-0F5E-471D-AFA2-1328A6EDBCED}" type="CELLRANGE">
+                    <a:fld id="{22E831A7-A476-48D2-B979-A4914ABB490B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7034,7 +7131,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7049,7 +7145,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D1A2907-D8EB-414D-BE5F-57CC5A9ADF11}" type="CELLRANGE">
+                    <a:fld id="{D26275A9-B826-4FD0-9602-F493632B2030}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7067,7 +7163,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7082,7 +7177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8EBC7BF-98F2-43E6-975D-C2CB15967729}" type="CELLRANGE">
+                    <a:fld id="{32E9CFE7-5B00-4863-8995-3C52BDFBADA2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7100,7 +7195,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7115,7 +7209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C268525-8F86-4710-BF13-AFC8B3B7856D}" type="CELLRANGE">
+                    <a:fld id="{14E60893-992A-4C8D-9D31-799F880D3B30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7133,7 +7227,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7148,7 +7241,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA7629EA-6015-42F8-912B-53343BDFD318}" type="CELLRANGE">
+                    <a:fld id="{B258B749-505C-4F97-9F17-4120C3B77651}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7166,7 +7259,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7181,7 +7273,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB220349-4FB7-4277-ADAC-1CB26F9A0C8A}" type="CELLRANGE">
+                    <a:fld id="{7F0CF75D-2A27-40ED-9E66-14C3A411CAB4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7199,7 +7291,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7214,7 +7305,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61316F62-4C46-4DFB-986B-5F889E86EA97}" type="CELLRANGE">
+                    <a:fld id="{929A2120-12A6-4AB0-8EC3-02595C95F45C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7232,7 +7323,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7247,7 +7337,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0812E4BE-0A96-4CA8-87D6-BBC89B9E8F6F}" type="CELLRANGE">
+                    <a:fld id="{DBF79EB5-E550-445D-84E6-05D3E2201D3E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7265,7 +7355,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7280,7 +7369,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA1D8C81-65EC-4647-AD6E-BB5F16D927FF}" type="CELLRANGE">
+                    <a:fld id="{B3415AF2-E3F7-4803-BA8F-3BE345A3B1BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7298,7 +7387,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7313,7 +7401,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56929E1E-7549-434A-85F6-A514E5582741}" type="CELLRANGE">
+                    <a:fld id="{8A45D555-B464-48AC-B7EE-055985C288A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7331,7 +7419,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7346,7 +7433,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27AC5CD5-0DC3-4568-BD9A-B2C5098A5E4A}" type="CELLRANGE">
+                    <a:fld id="{56B198A9-5DAB-4D85-9133-39A42A323512}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7364,7 +7451,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7379,7 +7465,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4892369C-367F-4BD1-8C0B-2C7666CF5A61}" type="CELLRANGE">
+                    <a:fld id="{B0227FB5-D747-4304-B3FB-F64163CFD9D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7397,7 +7483,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7412,7 +7497,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50042917-DF48-49AF-B201-7F1059D5A90D}" type="CELLRANGE">
+                    <a:fld id="{0341DFD4-34BD-4378-889E-5033E0931CBA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7430,7 +7515,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7445,7 +7529,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB2DEFB6-0947-43C0-9996-56747BDEBEB3}" type="CELLRANGE">
+                    <a:fld id="{2041A9D6-51C0-4048-94F7-9DDB8E1AEDE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9090,7 +9174,7 @@
     <tableColumn id="1" name="P0" dataCellStyle="Currency"/>
     <tableColumn id="2" name="P1" dataCellStyle="Currency"/>
     <tableColumn id="3" name="CashFlows" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="PeriodRet" dataDxfId="295" dataCellStyle="Percent">
+    <tableColumn id="4" name="PeriodRet" dataDxfId="312" dataCellStyle="Percent">
       <calculatedColumnFormula>($B2+$C2)/$A2-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9103,13 +9187,13 @@
   <autoFilter ref="N31:S35"/>
   <tableColumns count="6">
     <tableColumn id="1" name="State" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Probability" totalsRowDxfId="204" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="203" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="202" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="201" totalsRowDxfId="200" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowDxfId="221" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="220" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="219" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="218" totalsRowDxfId="217" dataCellStyle="Percent">
       <calculatedColumnFormula>($P32+$Q32)/160-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="199" totalsRowDxfId="198" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="216" totalsRowDxfId="215" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O32*$R32</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9121,22 +9205,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table378912" displayName="Table378912" ref="O38:V41" totalsRowCount="1">
   <autoFilter ref="O38:V40"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="197" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="196" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="195" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="194" totalsRowDxfId="193" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="214" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="213" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="212" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="211" totalsRowDxfId="210" dataCellStyle="Percent">
       <calculatedColumnFormula>($P39+$Q39)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="192" totalsRowDxfId="191" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="209" totalsRowDxfId="208" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O39*$R39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="190" totalsRowDxfId="189" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="207" totalsRowDxfId="206" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R39-$S$41,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="188" totalsRowDxfId="187" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="205" totalsRowDxfId="204" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T39*$O39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="186" totalsRowDxfId="185" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="203" totalsRowDxfId="202" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U41)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9149,53 +9233,53 @@
   <autoFilter ref="A1:T5"/>
   <tableColumns count="20">
     <tableColumn id="1" name="State" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="184" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Toyota" dataDxfId="183" totalsRowDxfId="182" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Walmart" dataDxfId="181" totalsRowDxfId="180" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Pfizer" dataDxfId="179" totalsRowDxfId="178" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Twted" totalsRowFunction="sum" dataDxfId="177" totalsRowDxfId="176" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="201" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Toyota" dataDxfId="200" totalsRowDxfId="199" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Walmart" dataDxfId="198" totalsRowDxfId="197" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Pfizer" dataDxfId="196" totalsRowDxfId="195" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Twted" totalsRowFunction="sum" dataDxfId="194" totalsRowDxfId="193" dataCellStyle="Percent">
       <calculatedColumnFormula>C2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WMTwted" totalsRowFunction="sum" dataDxfId="175" totalsRowDxfId="174" dataCellStyle="Percent">
+    <tableColumn id="7" name="WMTwted" totalsRowFunction="sum" dataDxfId="192" totalsRowDxfId="191" dataCellStyle="Percent">
       <calculatedColumnFormula>D2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PFZwted" totalsRowFunction="sum" dataDxfId="173" totalsRowDxfId="172" dataCellStyle="Percent">
+    <tableColumn id="8" name="PFZwted" totalsRowFunction="sum" dataDxfId="190" totalsRowDxfId="189" dataCellStyle="Percent">
       <calculatedColumnFormula>E2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Tvar" totalsRowFunction="sum" dataDxfId="171" totalsRowDxfId="170" dataCellStyle="Percent">
+    <tableColumn id="16" name="Tvar" totalsRowFunction="sum" dataDxfId="188" totalsRowDxfId="187" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(C2-F$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wvar" totalsRowFunction="sum" dataDxfId="169" totalsRowDxfId="168" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wvar" totalsRowFunction="sum" dataDxfId="186" totalsRowDxfId="185" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(D2-G$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Pvar" totalsRowFunction="sum" dataDxfId="167" totalsRowDxfId="166" dataCellStyle="Percent">
+    <tableColumn id="14" name="Pvar" totalsRowFunction="sum" dataDxfId="184" totalsRowDxfId="183" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(E2-H$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixT" dataDxfId="165" totalsRowDxfId="164" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixT" dataDxfId="182" totalsRowDxfId="181" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixWMT" dataDxfId="163" totalsRowDxfId="162" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixWMT" dataDxfId="180" totalsRowDxfId="179" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixPFZ" dataDxfId="161" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixPFZ" dataDxfId="178" dataCellStyle="Percent">
       <calculatedColumnFormula>1-L2-M2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="160" totalsRowDxfId="159" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="177" totalsRowDxfId="176" dataCellStyle="Percent">
       <calculatedColumnFormula>C2*L$2+D2*M$2+E2*N$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="158" totalsRowDxfId="157" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="175" totalsRowDxfId="174" dataCellStyle="Percent">
       <calculatedColumnFormula>O2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="MixVar" totalsRowFunction="sum" dataDxfId="156" totalsRowDxfId="155" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="17" name="MixVar" totalsRowFunction="sum" dataDxfId="173" totalsRowDxfId="172" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(O2-$P$6, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Wpcov" totalsRowFunction="sum" dataDxfId="154" totalsRowDxfId="153" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="18" name="Wpcov" totalsRowFunction="sum" dataDxfId="171" totalsRowDxfId="170" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(D2-G$6)*(E2-H$6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Tpcov" totalsRowFunction="sum" dataDxfId="152" totalsRowDxfId="151" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="19" name="Tpcov" totalsRowFunction="sum" dataDxfId="169" totalsRowDxfId="168" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(C2-F$6)*(E2-H$6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Twcov" totalsRowFunction="sum" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="20" name="Twcov" totalsRowFunction="sum" dataDxfId="167" totalsRowDxfId="166" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(C2-F$6)*(D2-G$6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9207,53 +9291,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1214" displayName="Table1214" ref="V1:AN5" totalsRowCount="1">
   <autoFilter ref="V1:AN4"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="148" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="147" totalsRowDxfId="146" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="145" totalsRowDxfId="144" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="143" totalsRowDxfId="142" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="141" totalsRowDxfId="140" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="165" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="164" totalsRowDxfId="163" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="162" totalsRowDxfId="161" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="160" totalsRowDxfId="159" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="158" totalsRowDxfId="157" dataCellStyle="Percent">
       <calculatedColumnFormula>W2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="139" totalsRowDxfId="138" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="156" totalsRowDxfId="155" dataCellStyle="Percent">
       <calculatedColumnFormula>X2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="137" totalsRowDxfId="136" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="154" totalsRowDxfId="153" dataCellStyle="Percent">
       <calculatedColumnFormula>Y2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="135" totalsRowDxfId="134" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="152" totalsRowDxfId="151" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(W2-Z$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="133" totalsRowDxfId="132" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(X2-AA$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="131" totalsRowDxfId="130" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="148" totalsRowDxfId="147" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(Y2-AB$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="129" totalsRowDxfId="128" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="146" totalsRowDxfId="145" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="127" totalsRowDxfId="126" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="144" totalsRowDxfId="143" dataCellStyle="Percent">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="125" totalsRowDxfId="124" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="142" totalsRowDxfId="141" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF2-AG2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="123" totalsRowDxfId="122" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="140" totalsRowDxfId="139" dataCellStyle="Percent">
       <calculatedColumnFormula>W2*AF$2+X2*AG$2+Y2*AH$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="121" totalsRowDxfId="120" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="138" totalsRowDxfId="137" dataCellStyle="Percent">
       <calculatedColumnFormula>AI2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="119" totalsRowDxfId="118" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="136" totalsRowDxfId="135" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(AI2-AJ$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="117" totalsRowDxfId="116" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="134" totalsRowDxfId="133" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(W2-Z$5)*(X2-AA$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="115" totalsRowDxfId="114" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="132" totalsRowDxfId="131" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(W2-Z$5)*(Y2-AB$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="130" totalsRowDxfId="129" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(X2-AA$5)*(Y2-AB$5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9266,9 +9350,9 @@
   <autoFilter ref="AP1:AS4"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Label" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="ExpRet" dataDxfId="111" totalsRowDxfId="110" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
-    <tableColumn id="3" name="Wt" totalsRowDxfId="109" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
-    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="107" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="2" name="ExpRet" dataDxfId="128" totalsRowDxfId="127" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
+    <tableColumn id="3" name="Wt" totalsRowDxfId="126" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
+    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="124" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>AQ2*AR2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9281,9 +9365,9 @@
   <autoFilter ref="AP8:AS11"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Label" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="ExpRet" dataDxfId="106" totalsRowDxfId="105" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
-    <tableColumn id="3" name="Wt" totalsRowDxfId="104" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
-    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="103" totalsRowDxfId="102" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="2" name="ExpRet" dataDxfId="123" totalsRowDxfId="122" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
+    <tableColumn id="3" name="Wt" totalsRowDxfId="121" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
+    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>AQ9*AR9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9297,8 +9381,8 @@
   <tableColumns count="9">
     <tableColumn id="1" name="Capital" dataCellStyle="Currency"/>
     <tableColumn id="2" name="Borrowed" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="LoanInt" dataDxfId="101" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Ret" dataDxfId="100" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="LoanInt" dataDxfId="118" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Ret" dataDxfId="117" dataCellStyle="Percent"/>
     <tableColumn id="5" name="TotInv">
       <calculatedColumnFormula>AU2+AV2</calculatedColumnFormula>
     </tableColumn>
@@ -9311,7 +9395,7 @@
     <tableColumn id="8" name="NetRetVal">
       <calculatedColumnFormula>AZ2-BA2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="RetRate" dataDxfId="99" dataCellStyle="Percent">
+    <tableColumn id="9" name="RetRate" dataDxfId="116" dataCellStyle="Percent">
       <calculatedColumnFormula>BB2/AU2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9323,53 +9407,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table121417" displayName="Table121417" ref="V9:AN13" totalsRowCount="1">
   <autoFilter ref="V9:AN12"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="98" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="97" totalsRowDxfId="96" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="95" totalsRowDxfId="94" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="93" totalsRowDxfId="92" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="91" totalsRowDxfId="90" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="115" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="114" totalsRowDxfId="113" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="112" totalsRowDxfId="111" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="110" totalsRowDxfId="109" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="107" dataCellStyle="Percent">
       <calculatedColumnFormula>W10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="89" totalsRowDxfId="88" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="105" dataCellStyle="Percent">
       <calculatedColumnFormula>X10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="87" totalsRowDxfId="86" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="103" dataCellStyle="Percent">
       <calculatedColumnFormula>Y10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="101" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(W10-Z$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="82" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="99" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(X10-AA$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="81" totalsRowDxfId="80" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="98" totalsRowDxfId="97" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(Y10-AB$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="79" totalsRowDxfId="78" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="96" totalsRowDxfId="95" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="77" totalsRowDxfId="76" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="94" totalsRowDxfId="93" dataCellStyle="Percent">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="75" totalsRowDxfId="74" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="92" totalsRowDxfId="91" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF10-AG10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="90" totalsRowDxfId="89" dataCellStyle="Percent">
       <calculatedColumnFormula>W10*AF$2+X10*AG$2+Y10*AH$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="88" totalsRowDxfId="87" dataCellStyle="Percent">
       <calculatedColumnFormula>AI10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(AI10-AJ$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="67" totalsRowDxfId="66" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(W10-Z$13)*(X10-AA$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="65" totalsRowDxfId="64" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(W10-Z$13)*(Y10-AB$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(X10-AA$13)*(Y10-AB$13)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9381,22 +9465,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="BE1:BQ2" totalsRowShown="0">
   <autoFilter ref="BE1:BQ2"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Jret" dataDxfId="61" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="Rret" dataDxfId="60" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Jret" dataDxfId="78" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="Rret" dataDxfId="77" dataCellStyle="Percent"/>
     <tableColumn id="3" name="Jwt"/>
     <tableColumn id="4" name="Rwt">
       <calculatedColumnFormula>1-BG2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="ExpRet" dataDxfId="59" dataCellStyle="Percent">
+    <tableColumn id="5" name="ExpRet" dataDxfId="76" dataCellStyle="Percent">
       <calculatedColumnFormula>BE2*BG2+BF2*BH2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Jvol" dataDxfId="58" dataCellStyle="Percent"/>
-    <tableColumn id="7" name="Rvol" dataDxfId="57" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Jrcorr" dataDxfId="56" dataCellStyle="Comma"/>
-    <tableColumn id="9" name="Jvar" dataDxfId="55" dataCellStyle="Percent">
+    <tableColumn id="6" name="Jvol" dataDxfId="75" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Rvol" dataDxfId="74" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Jrcorr" dataDxfId="73" dataCellStyle="Comma"/>
+    <tableColumn id="9" name="Jvar" dataDxfId="72" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BJ2,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Rvar" dataDxfId="54" dataCellStyle="Percent">
+    <tableColumn id="10" name="Rvar" dataDxfId="71" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BK2,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Jrcov">
@@ -9405,7 +9489,7 @@
     <tableColumn id="12" name="Jrvar">
       <calculatedColumnFormula>BM2*BG2*BG2+BN2*BH2*BH2+2*BG2*BH2*BO2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Jrvol" dataDxfId="53" dataCellStyle="Percent">
+    <tableColumn id="13" name="Jrvol" dataDxfId="70" dataCellStyle="Percent">
       <calculatedColumnFormula>SQRT(BP2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9417,24 +9501,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1820" displayName="Table1820" ref="BE6:BQ7" totalsRowShown="0">
   <autoFilter ref="BE6:BQ7"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Jret" dataDxfId="52" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="Rret" dataDxfId="51" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Jret" dataDxfId="69" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="Rret" dataDxfId="68" dataCellStyle="Percent"/>
     <tableColumn id="3" name="Jwt">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Rwt">
       <calculatedColumnFormula>1-BG7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="ExpRet" dataDxfId="50" dataCellStyle="Percent">
+    <tableColumn id="5" name="ExpRet" dataDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>BE7*BG7+BF7*BH7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Jvol" dataDxfId="49" dataCellStyle="Percent"/>
-    <tableColumn id="7" name="Rvol" dataDxfId="48" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Jrcorr" dataDxfId="47" dataCellStyle="Comma"/>
-    <tableColumn id="9" name="Jvar" dataDxfId="46" dataCellStyle="Percent">
+    <tableColumn id="6" name="Jvol" dataDxfId="66" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Rvol" dataDxfId="65" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Jrcorr" dataDxfId="64" dataCellStyle="Comma"/>
+    <tableColumn id="9" name="Jvar" dataDxfId="63" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BJ7,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Rvar" dataDxfId="45" dataCellStyle="Percent">
+    <tableColumn id="10" name="Rvar" dataDxfId="62" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BK7,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Jrcov">
@@ -9443,7 +9527,7 @@
     <tableColumn id="12" name="Jrvar">
       <calculatedColumnFormula>BM7*BG7*BG7+BN7*BH7*BH7+2*BG7*BH7*BO7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Jrvol" dataDxfId="44" dataCellStyle="Percent">
+    <tableColumn id="13" name="Jrvol" dataDxfId="61" dataCellStyle="Percent">
       <calculatedColumnFormula>SQRT(BP7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9456,20 +9540,20 @@
   <autoFilter ref="F1:L6"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="294" totalsRowDxfId="293" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="292" totalsRowDxfId="291" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="311" totalsRowDxfId="310" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="309" totalsRowDxfId="308" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="290" totalsRowDxfId="289" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="307" totalsRowDxfId="306" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$2:$H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="288" totalsRowDxfId="287" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="305" totalsRowDxfId="304" dataCellStyle="Percent">
       <calculatedColumnFormula>$I2-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="286" totalsRowDxfId="285" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="303" totalsRowDxfId="302" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$2:$H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="284" totalsRowDxfId="283" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="301" totalsRowDxfId="300" dataCellStyle="Percent">
       <calculatedColumnFormula>$K2-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9482,12 +9566,12 @@
   <autoFilter ref="BS1:BW4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Security" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Ret" dataDxfId="43" totalsRowDxfId="42" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="Invested" totalsRowFunction="sum" totalsRowDxfId="41" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Wt" dataDxfId="39" totalsRowDxfId="40" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="60" totalsRowDxfId="59" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="Invested" totalsRowFunction="sum" totalsRowDxfId="58" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Wt" dataDxfId="57" totalsRowDxfId="56" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>BU2/BU$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="WtdRet" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="WtdRet" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>BT2*BV2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9499,53 +9583,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table12141723" displayName="Table12141723" ref="V17:AN21" totalsRowCount="1">
   <autoFilter ref="V17:AN20"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="19" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="36" totalsRowDxfId="18" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="35" totalsRowDxfId="17" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="34" totalsRowDxfId="16" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="15" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="53" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="52" totalsRowDxfId="51" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="50" totalsRowDxfId="49" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="48" totalsRowDxfId="47" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="45" dataCellStyle="Percent">
       <calculatedColumnFormula>W18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="14" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="43" dataCellStyle="Percent">
       <calculatedColumnFormula>X18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="13" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Percent">
       <calculatedColumnFormula>Y18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="12" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(W18-Z$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="11" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(X18-AA$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="10" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(Y18-AB$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="22" totalsRowDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Percent">
       <calculatedColumnFormula>0.6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="21" totalsRowDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Percent">
       <calculatedColumnFormula>0.4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="30" totalsRowDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF18-AG18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="20" totalsRowDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Percent">
       <calculatedColumnFormula>W18*AF$18+X18*AG$18+Y18*AH$18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Percent">
       <calculatedColumnFormula>AI18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(AI18-AJ$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="3" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(W18-Z$21)*(X18-AA$21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="2" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(W18-Z$21)*(Y18-AB$21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(X18-AA$21)*(Y18-AB$21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9566,6 +9650,95 @@
 </table>
 </file>
 
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="A2:B3" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2" dataDxfId="16" dataCellStyle="Comma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table26" displayName="Table26" ref="A4:E7" totalsRowShown="0">
+  <autoFilter ref="A4:E7"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Investment"/>
+    <tableColumn id="2" name="Ret" dataDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="14" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="13" dataCellStyle="Comma">
+      <calculatedColumnFormula>C5*C5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Utility" dataDxfId="12" dataCellStyle="Comma">
+      <calculatedColumnFormula>B5-0.5*$B$2*D5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table2627" displayName="Table2627" ref="A9:E11" totalsRowShown="0">
+  <autoFilter ref="A9:E11"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Investment"/>
+    <tableColumn id="2" name="Ret" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="9" dataCellStyle="Comma">
+      <calculatedColumnFormula>C10*C10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Utility" dataDxfId="8" dataCellStyle="Comma">
+      <calculatedColumnFormula>B10-0.5*$B$2*D10</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table27" displayName="Table27" ref="G4:N6" totalsRowShown="0">
+  <autoFilter ref="G4:N6"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Investment"/>
+    <tableColumn id="2" name="W1" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="W2" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="P1" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="P2" dataDxfId="6" dataCellStyle="Comma">
+      <calculatedColumnFormula>1-J5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="U1" dataDxfId="5">
+      <calculatedColumnFormula>LN(H5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="U2">
+      <calculatedColumnFormula>LN(I5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="EU" dataDxfId="4">
+      <calculatedColumnFormula>J5*L5+K5*M5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table2624" displayName="Table2624" ref="A13:E16" totalsRowShown="0">
+  <autoFilter ref="A13:E16"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Investment"/>
+    <tableColumn id="2" name="Ret" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="1" dataCellStyle="Comma">
+      <calculatedColumnFormula>C14*C14</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Utility" dataDxfId="0" dataCellStyle="Comma">
+      <calculatedColumnFormula>B14-0.5*$B$2*D14</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="N1:S6" totalsRowCount="1">
   <autoFilter ref="N1:S5"/>
@@ -9574,10 +9747,10 @@
     <tableColumn id="2" name="Probability" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
     <tableColumn id="3" name="YrEndPrice" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
     <tableColumn id="4" name="CashFlow" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="282" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="5" name="Ret" dataDxfId="299" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>($P2+$Q2)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="281" totalsRowDxfId="280" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="298" totalsRowDxfId="297" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O2*$R2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9590,20 +9763,20 @@
   <autoFilter ref="F9:L12"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="296" totalsRowDxfId="295" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="294" totalsRowDxfId="293" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="292" totalsRowDxfId="291" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$10:$H10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="273" totalsRowDxfId="272" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="290" totalsRowDxfId="289" dataCellStyle="Percent">
       <calculatedColumnFormula>$I10-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="271" totalsRowDxfId="270" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="288" totalsRowDxfId="287" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$10:$H10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="269" totalsRowDxfId="268" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="286" totalsRowDxfId="285" dataCellStyle="Percent">
       <calculatedColumnFormula>$K10-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9615,22 +9788,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="O9:V13" totalsRowCount="1">
   <autoFilter ref="O9:V12"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="267" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="266" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="265" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="264" totalsRowDxfId="263" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="284" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="283" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="282" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="281" totalsRowDxfId="280" dataCellStyle="Percent">
       <calculatedColumnFormula>($P10+$Q10)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="262" totalsRowDxfId="261" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O10*$R10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="260" totalsRowDxfId="259" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R10-$S$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="258" totalsRowDxfId="257" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T10*$O10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="256" totalsRowDxfId="255" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="273" totalsRowDxfId="272" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U13)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9642,22 +9815,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table378" displayName="Table378" ref="O16:V20" totalsRowCount="1">
   <autoFilter ref="O16:V19"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="254" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="253" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="252" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="251" totalsRowDxfId="250" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="271" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="270" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="269" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="268" totalsRowDxfId="267" dataCellStyle="Percent">
       <calculatedColumnFormula>($P17+$Q17)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="249" totalsRowDxfId="248" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="266" totalsRowDxfId="265" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O17*$R17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="247" totalsRowDxfId="246" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="264" totalsRowDxfId="263" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R17-$S$20,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="245" totalsRowDxfId="244" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="262" totalsRowDxfId="261" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T17*$O17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="243" totalsRowDxfId="242" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="260" totalsRowDxfId="259" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U20)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9670,20 +9843,20 @@
   <autoFilter ref="F15:L18"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="241" totalsRowDxfId="240" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="239" totalsRowDxfId="238" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="258" totalsRowDxfId="257" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="256" totalsRowDxfId="255" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G16</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="237" totalsRowDxfId="236" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="254" totalsRowDxfId="253" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$16:$H16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="235" totalsRowDxfId="234" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="252" totalsRowDxfId="251" dataCellStyle="Percent">
       <calculatedColumnFormula>$I16-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="233" totalsRowDxfId="232" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="250" totalsRowDxfId="249" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$16:$H16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="231" totalsRowDxfId="230" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="248" totalsRowDxfId="247" dataCellStyle="Percent">
       <calculatedColumnFormula>$K16-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9695,22 +9868,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table3789" displayName="Table3789" ref="O23:V27" totalsRowCount="1">
   <autoFilter ref="O23:V26"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="229" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="228" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="227" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="226" totalsRowDxfId="225" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="246" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="245" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="244" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="243" totalsRowDxfId="242" dataCellStyle="Percent">
       <calculatedColumnFormula>($P24+$Q24)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="224" totalsRowDxfId="223" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="241" totalsRowDxfId="240" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O24*$R24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="222" totalsRowDxfId="221" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="239" totalsRowDxfId="238" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R24-$S$27,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="220" totalsRowDxfId="219" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="237" totalsRowDxfId="236" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T24*$O24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="218" totalsRowDxfId="217" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="235" totalsRowDxfId="234" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U27)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9723,20 +9896,20 @@
   <autoFilter ref="F23:L28"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="216" totalsRowDxfId="215" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="214" totalsRowDxfId="213" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="233" totalsRowDxfId="232" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="231" totalsRowDxfId="230" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="212" totalsRowDxfId="211" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="229" totalsRowDxfId="228" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$24:$H24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="210" totalsRowDxfId="209" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="227" totalsRowDxfId="226" dataCellStyle="Percent">
       <calculatedColumnFormula>$I24-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="208" totalsRowDxfId="207" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="225" totalsRowDxfId="224" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$24:$H24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="206" totalsRowDxfId="205" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="223" totalsRowDxfId="222" dataCellStyle="Percent">
       <calculatedColumnFormula>$K24-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11395,7 +11568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
+    <sheetView topLeftCell="BO1" workbookViewId="0">
       <selection activeCell="BY1" sqref="BY1"/>
     </sheetView>
   </sheetViews>
@@ -23795,4 +23968,330 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.7265625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="23"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="L4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="34">
+        <f t="shared" ref="D5:D7" si="0">C5*C5</f>
+        <v>0.09</v>
+      </c>
+      <c r="E5" s="34">
+        <f t="shared" ref="E5:E7" si="1">B5-0.5*$B$2*D5</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="1">
+        <v>150000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="J5" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="23">
+        <f>1-J5</f>
+        <v>0.5</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:M6" si="2">LN(H5)</f>
+        <v>11.918390573078392</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>10.819778284410283</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N6" si="3">J5*L5+K5*M5</f>
+        <v>11.369084428744337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="34">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="E6" s="34">
+        <f t="shared" si="1"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="1">
+        <v>125000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>55000</v>
+      </c>
+      <c r="J6" s="23">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K6" s="23">
+        <f>1-J6</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>11.736069016284437</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>10.915088464214607</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>11.462408832261161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="D7" s="34">
+        <f t="shared" si="0"/>
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="E7" s="34">
+        <f t="shared" si="1"/>
+        <v>-0.17500000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="34">
+        <f t="shared" ref="D10:D11" si="4">C10*C10</f>
+        <v>0.09</v>
+      </c>
+      <c r="E10" s="34">
+        <f t="shared" ref="E10:E11" si="5">B10-0.5*$B$2*D10</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="34">
+        <f t="shared" si="5"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D14" s="34">
+        <f t="shared" ref="D14:D16" si="6">C14*C14</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E14" s="34">
+        <f t="shared" ref="E14:E16" si="7">B14-0.5*$B$2*D14</f>
+        <v>2.4999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="34">
+        <f t="shared" si="6"/>
+        <v>0.09</v>
+      </c>
+      <c r="E15" s="34">
+        <f t="shared" si="7"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="D16" s="34">
+        <f t="shared" si="6"/>
+        <v>0.20250000000000001</v>
+      </c>
+      <c r="E16" s="34">
+        <f t="shared" si="7"/>
+        <v>-0.15500000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Portfolio Risk wk 4.
</commit_message>
<xml_diff>
--- a/ClassesTaken/Coursera/2016/InvManagementRice/02PortfolioRisk/PortfolioRisk.xlsx
+++ b/ClassesTaken/Coursera/2016/InvManagementRice/02PortfolioRisk/PortfolioRisk.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14928" windowHeight="8076" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14928" windowHeight="8076" tabRatio="702" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="wk01" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="covHw3data" sheetId="6" r:id="rId6"/>
     <sheet name="Hw3chart" sheetId="7" r:id="rId7"/>
     <sheet name="wk03" sheetId="8" r:id="rId8"/>
+    <sheet name="wk04" sheetId="9" r:id="rId9"/>
+    <sheet name="Felix" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="170">
   <si>
     <t>P0</t>
   </si>
@@ -465,12 +467,105 @@
   <si>
     <t>EU</t>
   </si>
+  <si>
+    <t>RiskFreeRate</t>
+  </si>
+  <si>
+    <t>SharpeRatio</t>
+  </si>
+  <si>
+    <t>ExpExcessRet</t>
+  </si>
+  <si>
+    <t>RiskyRet</t>
+  </si>
+  <si>
+    <t>RiskFreeRet</t>
+  </si>
+  <si>
+    <t>TargetRet</t>
+  </si>
+  <si>
+    <t>wRisky</t>
+  </si>
+  <si>
+    <t>RiskySD</t>
+  </si>
+  <si>
+    <t>TargetSD</t>
+  </si>
+  <si>
+    <t>riskySD</t>
+  </si>
+  <si>
+    <t>riskyRet</t>
+  </si>
+  <si>
+    <t>riskFreeRet</t>
+  </si>
+  <si>
+    <t>targSD</t>
+  </si>
+  <si>
+    <t>riskyWt</t>
+  </si>
+  <si>
+    <t>DivInv</t>
+  </si>
+  <si>
+    <t>FelixInv</t>
+  </si>
+  <si>
+    <t>DivWt</t>
+  </si>
+  <si>
+    <t>FelixWt</t>
+  </si>
+  <si>
+    <t>TotWt</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>Felix</t>
+  </si>
+  <si>
+    <t>Corr</t>
+  </si>
+  <si>
+    <t>Cov</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Wts</t>
+  </si>
+  <si>
+    <t>DivRet</t>
+  </si>
+  <si>
+    <t>GovRet</t>
+  </si>
+  <si>
+    <t>GovWt</t>
+  </si>
+  <si>
+    <t>PfRet</t>
+  </si>
+  <si>
+    <t>DivSD</t>
+  </si>
+  <si>
+    <t>PfSD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="10">
+  <numFmts count="12">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -481,6 +576,8 @@
     <numFmt numFmtId="169" formatCode="0.000000"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="0.00000%"/>
+    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -561,7 +658,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
@@ -597,6 +694,9 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -604,7 +704,190 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="313">
+  <dxfs count="353">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="170" formatCode="0.0000"/>
     </dxf>
@@ -4327,7 +4610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D5A4820-3F05-4964-9C96-B0972BAD64B8}" type="CELLRANGE">
+                    <a:fld id="{5546DD3E-6C38-4588-BC37-7394D37D3BB9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4360,7 +4643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EF7C3E9-5C0B-4DFD-A95F-46B9E41C33A0}" type="CELLRANGE">
+                    <a:fld id="{6F550AC5-ED97-4A3C-82BB-CBBDD1A15E8A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4378,6 +4661,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4392,7 +4676,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C59BC26-9D00-43EA-87EB-742CD8CB0D41}" type="CELLRANGE">
+                    <a:fld id="{E469D964-7C07-458C-944B-143E31EB9C20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4410,6 +4694,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4424,7 +4709,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49928F6F-AF45-48CF-8BB0-6624BB8B3B6B}" type="CELLRANGE">
+                    <a:fld id="{D0239713-D04C-47A9-8937-BD9B479F5A62}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4442,6 +4727,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4456,7 +4742,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0948C18-DD95-4EFC-838A-47C97C8F07C6}" type="CELLRANGE">
+                    <a:fld id="{5FE7718F-7923-41A4-A39A-79130B55D7C2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4474,6 +4760,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4488,7 +4775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A022E7B-DFF9-41E4-BE15-F12E2C1AB623}" type="CELLRANGE">
+                    <a:fld id="{0634DD1D-CDD0-4C5A-99FF-7AAC238C69A3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4506,6 +4793,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4520,7 +4808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F7FABB3-FFB1-4067-9252-96B49D7E670C}" type="CELLRANGE">
+                    <a:fld id="{B86A0263-2A9B-43A7-A2AF-6774B48374A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4538,6 +4826,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4552,7 +4841,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D948FB4B-10E1-4E7C-B61A-C6CB4BD13FA5}" type="CELLRANGE">
+                    <a:fld id="{F5F8506E-6D4D-41F7-9DAD-AC0CF962AE88}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4570,6 +4859,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4584,7 +4874,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2054C994-9C41-434E-B854-1E05ED7A407E}" type="CELLRANGE">
+                    <a:fld id="{CBEB418D-7E5F-415F-8487-89721300A9DC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4602,6 +4892,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4616,7 +4907,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29A048BF-8A5E-46F1-923C-198055E499DD}" type="CELLRANGE">
+                    <a:fld id="{92CDFA4F-D3CF-4F25-B786-D636DDEA1754}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4634,6 +4925,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4648,7 +4940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A9162AA-445A-4636-B759-D5D21CC699AA}" type="CELLRANGE">
+                    <a:fld id="{94269597-8AA6-4598-A1A8-BB6F4A355220}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4666,6 +4958,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4680,7 +4973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C566B814-0FB4-48CE-AB65-33165D78FCF1}" type="CELLRANGE">
+                    <a:fld id="{224CFF0C-FB32-4206-AC91-18C503CC4C0C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4698,6 +4991,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4712,7 +5006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB123880-EEA9-4A57-BF73-71769560F4E5}" type="CELLRANGE">
+                    <a:fld id="{B8ACF232-282A-422E-8651-9D789547E117}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4730,6 +5024,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4744,7 +5039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBDA353E-6AF4-45EC-B4EB-93B64024D538}" type="CELLRANGE">
+                    <a:fld id="{E5EDD2AD-68CD-4FE2-9072-2DC399E195AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4762,6 +5057,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4776,7 +5072,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82019887-4446-4352-B922-315327FBA133}" type="CELLRANGE">
+                    <a:fld id="{725B8A45-3341-4C0B-9490-01B87C76689A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4794,6 +5090,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4808,7 +5105,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93EFA4E3-F765-45F6-8AEB-665908864B2D}" type="CELLRANGE">
+                    <a:fld id="{9B84BC46-FCDA-4A0A-B4FB-4755FDAF9A2C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4826,6 +5123,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4840,7 +5138,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9840E6BB-4E9C-47A3-BEA9-0F81B3240122}" type="CELLRANGE">
+                    <a:fld id="{E00DB2C8-6778-464E-9363-4BFE8281E5BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4858,6 +5156,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4872,7 +5171,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{864F5460-87AA-4BB5-B2D2-F707B3C3D1BC}" type="CELLRANGE">
+                    <a:fld id="{7ABCEC7C-712D-4325-9EE2-A64177D8BE8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4890,6 +5189,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4904,7 +5204,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{266F8357-D943-43AA-84D9-B15370FF64B7}" type="CELLRANGE">
+                    <a:fld id="{EB59660D-C0E9-40AF-9CB7-256035B2F10C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4922,6 +5222,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4936,7 +5237,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF3DF3BC-D7E3-4B51-AB3C-24B3CA5B957F}" type="CELLRANGE">
+                    <a:fld id="{8BDC5895-F53B-4592-AA54-1D20900C06CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4954,6 +5255,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4968,7 +5270,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91EB5A47-469A-4E59-9839-15A0FF14440B}" type="CELLRANGE">
+                    <a:fld id="{982D65CF-4292-4AE3-AB32-150DF73A8F02}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4986,6 +5288,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5000,7 +5303,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58F8B8D5-1F8C-4786-8D9D-4B45F0E0A7B1}" type="CELLRANGE">
+                    <a:fld id="{AE9B8273-C2A8-4EE0-9B41-60352A5B7AB8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5018,6 +5321,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5032,7 +5336,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B910AE8-7E10-47F8-9AA9-10A3E5F43E24}" type="CELLRANGE">
+                    <a:fld id="{471D99AE-A4B5-407B-A7A1-4E65A4F0FA30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5050,6 +5354,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5064,7 +5369,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0229948-1863-4788-8636-2FA751759F93}" type="CELLRANGE">
+                    <a:fld id="{5258CF8A-CD79-4410-A9EC-A8A86F3B7D36}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5082,6 +5387,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5096,7 +5402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E204CC38-1EBD-43D4-A42E-93BA5332F365}" type="CELLRANGE">
+                    <a:fld id="{3C3E9BE3-415D-41A6-968E-ABF8B674BF2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5114,6 +5420,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5128,7 +5435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F1F4B1B-748C-4744-B76D-A3EE34C8664E}" type="CELLRANGE">
+                    <a:fld id="{A18004C3-4763-4F2C-8AF9-3F431DAFFB86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5146,6 +5453,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5160,7 +5468,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C421093-8381-4A02-9C03-710204B3ABD0}" type="CELLRANGE">
+                    <a:fld id="{B851863A-1C76-4218-8511-6D75C5DDD04E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5178,6 +5486,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5192,7 +5501,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1EF76E3-AA06-490E-83B1-9CE6266E5F92}" type="CELLRANGE">
+                    <a:fld id="{B10E785F-836E-4973-9851-69755D9EC970}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5210,6 +5519,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5224,7 +5534,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECF717A1-558B-4308-BBC3-8E49459DC25E}" type="CELLRANGE">
+                    <a:fld id="{A5DB148C-6FD6-492F-926E-A807B66ED9A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5242,6 +5552,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5256,7 +5567,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C48E8CA6-9179-488E-BA0C-431DDC68010E}" type="CELLRANGE">
+                    <a:fld id="{FF892B70-19F8-40CD-AF54-42BFBCAD4F5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5274,6 +5585,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5288,7 +5600,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7697E68E-B9E0-4B1A-856B-DC27D572B609}" type="CELLRANGE">
+                    <a:fld id="{2662B45F-FDB5-4077-AEFA-A4C20E7BBF19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5306,6 +5618,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5320,7 +5633,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E1081374-AB01-4655-896D-8F52EAC413E1}" type="CELLRANGE">
+                    <a:fld id="{A9803C19-D934-4BDD-AF92-D038EFE11B0B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5338,6 +5651,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5352,7 +5666,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2569A406-9D96-4163-9D7D-FFBB3A45E5B6}" type="CELLRANGE">
+                    <a:fld id="{8B5F7519-2D4A-4F81-977F-629BFAA1DF8F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5370,6 +5684,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5384,7 +5699,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26CDA9DF-6167-4F27-9C24-1937736D76DF}" type="CELLRANGE">
+                    <a:fld id="{13DE5BA7-24AF-479F-ADD7-D580CBCF23E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5402,6 +5717,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5416,7 +5732,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A61BA4FB-215D-4593-A67F-6BC82F1F8ADD}" type="CELLRANGE">
+                    <a:fld id="{86A922EC-BE03-4DDD-832B-56BA766A74E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5434,6 +5750,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5448,7 +5765,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F75F754-F24A-4843-8E6D-0F2A0EC60209}" type="CELLRANGE">
+                    <a:fld id="{FFB47D17-5EEF-4987-BB11-36913091F9FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5466,6 +5783,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5480,7 +5798,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C6381FC-5733-4BA5-AF44-D38AD93E4F8B}" type="CELLRANGE">
+                    <a:fld id="{849B78C2-D93C-4225-8097-C04C8C3950BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5498,6 +5816,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5512,7 +5831,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C9FEF8E-8838-410C-822D-10F5F230388B}" type="CELLRANGE">
+                    <a:fld id="{14FD3B05-3183-48B4-8656-0E26579BA802}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5530,6 +5849,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5544,7 +5864,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E1467B2F-19D7-4E2A-930B-4B7C3A40DFCF}" type="CELLRANGE">
+                    <a:fld id="{0B301E80-A101-415E-A9C7-F7D0EB6B0823}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5562,6 +5882,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5576,7 +5897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51DA1B63-8AA8-44EA-B63C-895D6761BACB}" type="CELLRANGE">
+                    <a:fld id="{BC159138-0EDA-41AB-A95B-583B794C9EFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5594,6 +5915,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5608,7 +5930,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F058E486-CECC-40F2-8D83-346DE3DF0AF0}" type="CELLRANGE">
+                    <a:fld id="{FB551726-75AF-425B-8960-B189C8FF3FAE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5626,6 +5948,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5640,7 +5963,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D00FC07-7365-4853-A951-BEA3E49430DF}" type="CELLRANGE">
+                    <a:fld id="{02C38043-120D-426B-8833-2B48DD219129}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5658,6 +5981,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5672,7 +5996,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41919063-E0E6-4D09-AABD-51C60858ABD1}" type="CELLRANGE">
+                    <a:fld id="{EC697B59-A13B-49CE-8EC4-1B078B03A1AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5690,6 +6014,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5704,7 +6029,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{495AEF83-887D-4441-BAFF-9A3470FC3796}" type="CELLRANGE">
+                    <a:fld id="{AD33B331-044E-4DEC-9135-0CCCFC2EEFE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5722,6 +6047,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5736,7 +6062,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7CF26D3-DCE9-4480-9A35-B483E60B414A}" type="CELLRANGE">
+                    <a:fld id="{2071E286-9B08-4BE6-B735-2B39545DCB4F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5754,6 +6080,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5768,7 +6095,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55610D42-5CC7-4069-976A-309AA281BE67}" type="CELLRANGE">
+                    <a:fld id="{CF9000AA-D817-4682-85ED-27928F44D021}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5786,6 +6113,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5800,7 +6128,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C0AB8FB-1566-46FC-B4E6-D85B0F39F82F}" type="CELLRANGE">
+                    <a:fld id="{23150F83-8A76-442F-B288-03F9841E8219}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5818,6 +6146,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5832,7 +6161,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21B414A3-CEFE-41F0-B781-CB6EBC37602B}" type="CELLRANGE">
+                    <a:fld id="{B5B0B3A1-AC06-4C1F-BDA8-84308A1B6901}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5850,6 +6179,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5864,7 +6194,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56305D20-94EF-4F2F-A0A7-A399CCF6199B}" type="CELLRANGE">
+                    <a:fld id="{EFD6BFB0-DC42-48E0-BD8D-D201E621B3E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5882,6 +6212,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5896,7 +6227,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6067DE17-C64B-4FA9-BF47-6FC244B5E0AA}" type="CELLRANGE">
+                    <a:fld id="{CE74049C-6365-4578-A979-137C89BC25E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5914,6 +6245,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5928,7 +6260,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CC69B2D-59BB-496C-8837-96FE3FA7A0BD}" type="CELLRANGE">
+                    <a:fld id="{319B60DB-4495-4981-959E-ACF78C754C47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5961,7 +6293,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA1D1933-8255-4587-828F-DAE0CD56072B}" type="CELLRANGE">
+                    <a:fld id="{16C070FF-F401-4D7F-8E4A-2ECED647E329}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5979,6 +6311,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5993,7 +6326,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4468F7A5-D9C2-44A9-A288-76FD6A9EA9D0}" type="CELLRANGE">
+                    <a:fld id="{34BFC6B0-A5C6-42D4-A369-315FE5188427}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6011,6 +6344,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6025,7 +6359,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F64091AF-1066-405A-B720-206CA90307A3}" type="CELLRANGE">
+                    <a:fld id="{DAF444B0-7668-42FE-B392-C92C3E77EB76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6043,6 +6377,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6057,7 +6392,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22D97079-61EB-41CA-9C10-530E6C3C065A}" type="CELLRANGE">
+                    <a:fld id="{F67A0D88-F5A0-4174-A9D5-2FDF3A58A7E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6075,6 +6410,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6089,7 +6425,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34E2345B-B469-4377-B04B-B3F8D8060B99}" type="CELLRANGE">
+                    <a:fld id="{599B789E-E7E1-484B-80A3-2F67ACF5D5AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6107,6 +6443,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6121,7 +6458,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ABB5E11F-C6D5-4E6C-BB81-F345DB8964AF}" type="CELLRANGE">
+                    <a:fld id="{A7A8FDE4-D3F5-4A32-A0E7-7F8E4C66C692}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6139,6 +6476,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6153,7 +6491,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1FB38142-9A1F-4E7B-8D18-8578FFDDA748}" type="CELLRANGE">
+                    <a:fld id="{2CBB1A62-1848-4422-8F08-C88B04B50BD1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6171,6 +6509,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6185,7 +6524,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5D9CB81-EE10-4FEB-84BC-8262E68B875E}" type="CELLRANGE">
+                    <a:fld id="{CD196D26-BF39-4F37-A722-3C8B73D89F3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6203,6 +6542,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6217,7 +6557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5C24F7E-A335-48A6-B4CD-1A2231B8D84B}" type="CELLRANGE">
+                    <a:fld id="{CF562CAF-0615-4AFA-A9AC-D794A93A0E92}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6235,6 +6575,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6249,7 +6590,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17B44E5D-5BEF-4DB9-A678-AAE2EED31641}" type="CELLRANGE">
+                    <a:fld id="{86F521B4-C975-47F2-B001-6C29C41839E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6267,6 +6608,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6281,7 +6623,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDBC9B43-421C-4C1A-82A0-2EC57000B919}" type="CELLRANGE">
+                    <a:fld id="{B6D93F50-D0AB-4845-B2F4-5A41BCA4780C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6299,6 +6641,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6313,7 +6656,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{351BF981-2A76-4BFB-89DB-1970B94F27B6}" type="CELLRANGE">
+                    <a:fld id="{7A14C5AB-62A0-4302-88C0-AAFFF5A4D9F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6331,6 +6674,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6345,7 +6689,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DABD37D-4DEC-40C8-A966-8E11C26E97D1}" type="CELLRANGE">
+                    <a:fld id="{F8C95B39-3F4C-45EA-9AAF-1D30C6DCBBD8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6363,6 +6707,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6377,7 +6722,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19C9FA57-E595-4606-8A6D-5FC6C50262BE}" type="CELLRANGE">
+                    <a:fld id="{2F0ABDE2-5FA1-456F-A76C-31B77AC2DA72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6395,6 +6740,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6409,7 +6755,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC035C02-650E-4733-B144-90FB15DBD353}" type="CELLRANGE">
+                    <a:fld id="{40728121-34E1-4ECB-B2DD-15461F552AA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6427,6 +6773,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6441,7 +6788,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3A41DDB-3C1C-49F2-AC32-F409CB48A81C}" type="CELLRANGE">
+                    <a:fld id="{3463F136-4702-408B-9C3C-404EB2C6389D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6459,6 +6806,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6473,7 +6821,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{160A819D-0064-411E-B95A-366D0F21C5BD}" type="CELLRANGE">
+                    <a:fld id="{60217F84-6FB4-43F9-9D7E-008993D9EE59}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6491,6 +6839,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6505,7 +6854,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25934EE9-18FF-4D91-8595-45849EB98525}" type="CELLRANGE">
+                    <a:fld id="{12587F89-4787-40CE-9C2A-FB16455AF63D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6523,6 +6872,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6537,7 +6887,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B7B8B5E-614F-47F0-84D7-62371EE9AA9A}" type="CELLRANGE">
+                    <a:fld id="{36C61D10-5241-421B-8946-B796B2BDE709}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6555,6 +6905,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6569,7 +6920,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0F029D3-F6F7-4ABC-860D-6D6709803C80}" type="CELLRANGE">
+                    <a:fld id="{135C79AF-F7ED-4EE6-8630-A538D6279F88}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6587,6 +6938,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6601,7 +6953,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{397BB740-7000-46AF-AB9C-F4A3A2CCF2FA}" type="CELLRANGE">
+                    <a:fld id="{4C9520DB-8BC7-4590-A9E8-57DABFF1AB05}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6619,6 +6971,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6633,7 +6986,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{821248B2-3E06-46E0-98F2-778385FA03B7}" type="CELLRANGE">
+                    <a:fld id="{58173E57-200F-4E54-AF12-EE6592436E99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6651,6 +7004,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6665,7 +7019,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A203DE8-A5E3-4ADA-A99D-1B3AA2848B02}" type="CELLRANGE">
+                    <a:fld id="{59A55068-7B23-4A79-8156-23EC562B7A5C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6683,6 +7037,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6697,7 +7052,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7202B26D-3070-4B86-8F33-1F2CC1BD2F48}" type="CELLRANGE">
+                    <a:fld id="{B7403EF6-64A9-410E-B1E2-37EB587C193D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6715,6 +7070,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6729,7 +7085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AEC927C-6952-4D3E-822C-931218B99934}" type="CELLRANGE">
+                    <a:fld id="{AB663849-4653-41E1-AD8B-E2DCCF4B4D67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6747,6 +7103,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6761,7 +7118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04CE457D-E011-480F-911D-514D3190E39F}" type="CELLRANGE">
+                    <a:fld id="{D3EA022C-8BE3-4D47-8BF6-582FD3B2B85A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6779,6 +7136,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6793,7 +7151,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4964FC94-B544-4934-9D01-AF12B495EC4F}" type="CELLRANGE">
+                    <a:fld id="{0CAF838E-881A-4926-8632-C7928F818505}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6811,6 +7169,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6825,7 +7184,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{27222FFE-AA8E-4345-A456-F0FA83DFCDB2}" type="CELLRANGE">
+                    <a:fld id="{DC3B0EA7-E9BB-4246-A670-EC2DC8230C03}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6843,6 +7202,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6857,7 +7217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1ABAD332-269B-4F4C-A332-F86E20A6A883}" type="CELLRANGE">
+                    <a:fld id="{582A26FE-7D19-46A6-8AEC-3B07CEAB8D99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6875,6 +7235,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6889,7 +7250,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E59BE2D-0DFE-4DD9-A3BB-C23ED465E001}" type="CELLRANGE">
+                    <a:fld id="{9CEE8AB5-5F39-41B4-B4AD-44C2771B37A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6907,6 +7268,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6921,7 +7283,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC5E4F2D-B3E4-4B27-8033-2B95E3C9116A}" type="CELLRANGE">
+                    <a:fld id="{19D6A829-DA3D-478A-8EC7-03FDFFE4FE4E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6939,6 +7301,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6953,7 +7316,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B72154C-5745-4E4A-9285-5B2F09F5D830}" type="CELLRANGE">
+                    <a:fld id="{2CD9AD94-227E-473A-A556-11427797C00D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6971,6 +7334,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6985,7 +7349,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{797DD8E5-FE59-4BCB-85EF-868F1D50F57D}" type="CELLRANGE">
+                    <a:fld id="{E143CD50-B47B-40CD-AECF-8B6D14153590}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7003,6 +7367,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7017,7 +7382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0048AB6B-7E45-4BCF-881E-5E0C8FE1CE6A}" type="CELLRANGE">
+                    <a:fld id="{A23CEAB5-62FE-449E-B198-BEC8213A64D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7035,6 +7400,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7049,7 +7415,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85CC1774-FDBD-46DA-81E2-0B4BE25EEFE4}" type="CELLRANGE">
+                    <a:fld id="{14B8C6E1-7D34-42A9-A94D-9D3BB9FFC5D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7067,6 +7433,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7081,7 +7448,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F64B4BD-E220-41F4-8BE2-7485D7F164A7}" type="CELLRANGE">
+                    <a:fld id="{F7B7C73E-A02C-4177-848D-52E30E2E31D2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7099,6 +7466,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7113,7 +7481,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22E831A7-A476-48D2-B979-A4914ABB490B}" type="CELLRANGE">
+                    <a:fld id="{C5C501B8-164A-4F18-8E0F-6E5C31F196EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7131,6 +7499,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7145,7 +7514,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D26275A9-B826-4FD0-9602-F493632B2030}" type="CELLRANGE">
+                    <a:fld id="{F8847FB3-64CA-49AA-99FA-AF994A9210CF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7163,6 +7532,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7177,7 +7547,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32E9CFE7-5B00-4863-8995-3C52BDFBADA2}" type="CELLRANGE">
+                    <a:fld id="{6BB4EDD9-8C50-4C72-AA44-5D9F17580F88}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7195,6 +7565,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7209,7 +7580,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14E60893-992A-4C8D-9D31-799F880D3B30}" type="CELLRANGE">
+                    <a:fld id="{361FE5B0-19F2-4857-B02D-F69C687AB13B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7227,6 +7598,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7241,7 +7613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B258B749-505C-4F97-9F17-4120C3B77651}" type="CELLRANGE">
+                    <a:fld id="{9D3E5009-7F4F-4CFC-8906-2137E3CC5937}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7259,6 +7631,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7273,7 +7646,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F0CF75D-2A27-40ED-9E66-14C3A411CAB4}" type="CELLRANGE">
+                    <a:fld id="{D906CB0A-1F33-4239-984D-2EF36013D3DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7291,6 +7664,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7305,7 +7679,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{929A2120-12A6-4AB0-8EC3-02595C95F45C}" type="CELLRANGE">
+                    <a:fld id="{98D1921D-19CE-45DC-8CA8-F083869FE7F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7323,6 +7697,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7337,7 +7712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBF79EB5-E550-445D-84E6-05D3E2201D3E}" type="CELLRANGE">
+                    <a:fld id="{39B36489-8B10-441B-99F5-B139A6261B86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7355,6 +7730,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7369,7 +7745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3415AF2-E3F7-4803-BA8F-3BE345A3B1BA}" type="CELLRANGE">
+                    <a:fld id="{2A7365C9-FC21-4310-8A59-E223CC18567A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7387,6 +7763,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7401,7 +7778,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A45D555-B464-48AC-B7EE-055985C288A9}" type="CELLRANGE">
+                    <a:fld id="{2FE51C8B-D905-4213-924A-6E72E9A43E13}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7419,6 +7796,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7433,7 +7811,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56B198A9-5DAB-4D85-9133-39A42A323512}" type="CELLRANGE">
+                    <a:fld id="{DFD286E3-2D02-4B36-9E6A-6E59260C578F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7451,6 +7829,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7465,7 +7844,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0227FB5-D747-4304-B3FB-F64163CFD9D7}" type="CELLRANGE">
+                    <a:fld id="{31072938-8E44-429D-B86B-B42DC30C485D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7483,6 +7862,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7497,7 +7877,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0341DFD4-34BD-4378-889E-5033E0931CBA}" type="CELLRANGE">
+                    <a:fld id="{9EDEC461-4770-43DC-8CCA-EE53DEAA9BA6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7515,6 +7895,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -7529,7 +7910,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2041A9D6-51C0-4048-94F7-9DDB8E1AEDE8}" type="CELLRANGE">
+                    <a:fld id="{8511CF7D-C8B3-477D-94F2-4442C0BAB84E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9174,7 +9555,7 @@
     <tableColumn id="1" name="P0" dataCellStyle="Currency"/>
     <tableColumn id="2" name="P1" dataCellStyle="Currency"/>
     <tableColumn id="3" name="CashFlows" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="PeriodRet" dataDxfId="312" dataCellStyle="Percent">
+    <tableColumn id="4" name="PeriodRet" dataDxfId="352" dataCellStyle="Percent">
       <calculatedColumnFormula>($B2+$C2)/$A2-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9187,13 +9568,13 @@
   <autoFilter ref="N31:S35"/>
   <tableColumns count="6">
     <tableColumn id="1" name="State" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Probability" totalsRowDxfId="221" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="220" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="219" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="218" totalsRowDxfId="217" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowDxfId="261" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="260" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="259" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="258" totalsRowDxfId="257" dataCellStyle="Percent">
       <calculatedColumnFormula>($P32+$Q32)/160-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="216" totalsRowDxfId="215" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="256" totalsRowDxfId="255" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O32*$R32</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9205,22 +9586,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table378912" displayName="Table378912" ref="O38:V41" totalsRowCount="1">
   <autoFilter ref="O38:V40"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="214" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="213" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="212" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="211" totalsRowDxfId="210" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="254" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="253" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="252" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="251" totalsRowDxfId="250" dataCellStyle="Percent">
       <calculatedColumnFormula>($P39+$Q39)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="209" totalsRowDxfId="208" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="249" totalsRowDxfId="248" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O39*$R39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="207" totalsRowDxfId="206" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="247" totalsRowDxfId="246" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R39-$S$41,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="205" totalsRowDxfId="204" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="245" totalsRowDxfId="244" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T39*$O39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="203" totalsRowDxfId="202" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="243" totalsRowDxfId="242" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U41)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9233,53 +9614,53 @@
   <autoFilter ref="A1:T5"/>
   <tableColumns count="20">
     <tableColumn id="1" name="State" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="201" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Toyota" dataDxfId="200" totalsRowDxfId="199" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Walmart" dataDxfId="198" totalsRowDxfId="197" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Pfizer" dataDxfId="196" totalsRowDxfId="195" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Twted" totalsRowFunction="sum" dataDxfId="194" totalsRowDxfId="193" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="241" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Toyota" dataDxfId="240" totalsRowDxfId="239" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Walmart" dataDxfId="238" totalsRowDxfId="237" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Pfizer" dataDxfId="236" totalsRowDxfId="235" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Twted" totalsRowFunction="sum" dataDxfId="234" totalsRowDxfId="233" dataCellStyle="Percent">
       <calculatedColumnFormula>C2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WMTwted" totalsRowFunction="sum" dataDxfId="192" totalsRowDxfId="191" dataCellStyle="Percent">
+    <tableColumn id="7" name="WMTwted" totalsRowFunction="sum" dataDxfId="232" totalsRowDxfId="231" dataCellStyle="Percent">
       <calculatedColumnFormula>D2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PFZwted" totalsRowFunction="sum" dataDxfId="190" totalsRowDxfId="189" dataCellStyle="Percent">
+    <tableColumn id="8" name="PFZwted" totalsRowFunction="sum" dataDxfId="230" totalsRowDxfId="229" dataCellStyle="Percent">
       <calculatedColumnFormula>E2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Tvar" totalsRowFunction="sum" dataDxfId="188" totalsRowDxfId="187" dataCellStyle="Percent">
+    <tableColumn id="16" name="Tvar" totalsRowFunction="sum" dataDxfId="228" totalsRowDxfId="227" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(C2-F$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wvar" totalsRowFunction="sum" dataDxfId="186" totalsRowDxfId="185" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wvar" totalsRowFunction="sum" dataDxfId="226" totalsRowDxfId="225" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(D2-G$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Pvar" totalsRowFunction="sum" dataDxfId="184" totalsRowDxfId="183" dataCellStyle="Percent">
+    <tableColumn id="14" name="Pvar" totalsRowFunction="sum" dataDxfId="224" totalsRowDxfId="223" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(E2-H$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixT" dataDxfId="182" totalsRowDxfId="181" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixT" dataDxfId="222" totalsRowDxfId="221" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixWMT" dataDxfId="180" totalsRowDxfId="179" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixWMT" dataDxfId="220" totalsRowDxfId="219" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixPFZ" dataDxfId="178" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixPFZ" dataDxfId="218" dataCellStyle="Percent">
       <calculatedColumnFormula>1-L2-M2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="177" totalsRowDxfId="176" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="217" totalsRowDxfId="216" dataCellStyle="Percent">
       <calculatedColumnFormula>C2*L$2+D2*M$2+E2*N$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="175" totalsRowDxfId="174" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="215" totalsRowDxfId="214" dataCellStyle="Percent">
       <calculatedColumnFormula>O2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="MixVar" totalsRowFunction="sum" dataDxfId="173" totalsRowDxfId="172" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="17" name="MixVar" totalsRowFunction="sum" dataDxfId="213" totalsRowDxfId="212" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(O2-$P$6, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Wpcov" totalsRowFunction="sum" dataDxfId="171" totalsRowDxfId="170" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="18" name="Wpcov" totalsRowFunction="sum" dataDxfId="211" totalsRowDxfId="210" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(D2-G$6)*(E2-H$6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Tpcov" totalsRowFunction="sum" dataDxfId="169" totalsRowDxfId="168" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="19" name="Tpcov" totalsRowFunction="sum" dataDxfId="209" totalsRowDxfId="208" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(C2-F$6)*(E2-H$6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Twcov" totalsRowFunction="sum" dataDxfId="167" totalsRowDxfId="166" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="20" name="Twcov" totalsRowFunction="sum" dataDxfId="207" totalsRowDxfId="206" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(C2-F$6)*(D2-G$6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9291,53 +9672,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1214" displayName="Table1214" ref="V1:AN5" totalsRowCount="1">
   <autoFilter ref="V1:AN4"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="165" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="164" totalsRowDxfId="163" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="162" totalsRowDxfId="161" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="160" totalsRowDxfId="159" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="158" totalsRowDxfId="157" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="205" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="204" totalsRowDxfId="203" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="202" totalsRowDxfId="201" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="200" totalsRowDxfId="199" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="198" totalsRowDxfId="197" dataCellStyle="Percent">
       <calculatedColumnFormula>W2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="156" totalsRowDxfId="155" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="196" totalsRowDxfId="195" dataCellStyle="Percent">
       <calculatedColumnFormula>X2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="154" totalsRowDxfId="153" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="194" totalsRowDxfId="193" dataCellStyle="Percent">
       <calculatedColumnFormula>Y2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="152" totalsRowDxfId="151" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="192" totalsRowDxfId="191" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(W2-Z$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="190" totalsRowDxfId="189" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(X2-AA$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="148" totalsRowDxfId="147" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="188" totalsRowDxfId="187" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(Y2-AB$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="146" totalsRowDxfId="145" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="186" totalsRowDxfId="185" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="144" totalsRowDxfId="143" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="184" totalsRowDxfId="183" dataCellStyle="Percent">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="142" totalsRowDxfId="141" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="182" totalsRowDxfId="181" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF2-AG2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="140" totalsRowDxfId="139" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="180" totalsRowDxfId="179" dataCellStyle="Percent">
       <calculatedColumnFormula>W2*AF$2+X2*AG$2+Y2*AH$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="138" totalsRowDxfId="137" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="178" totalsRowDxfId="177" dataCellStyle="Percent">
       <calculatedColumnFormula>AI2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="136" totalsRowDxfId="135" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="176" totalsRowDxfId="175" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(AI2-AJ$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="134" totalsRowDxfId="133" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="174" totalsRowDxfId="173" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(W2-Z$5)*(X2-AA$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="132" totalsRowDxfId="131" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="172" totalsRowDxfId="171" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(W2-Z$5)*(Y2-AB$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="130" totalsRowDxfId="129" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="170" totalsRowDxfId="169" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(X2-AA$5)*(Y2-AB$5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9350,9 +9731,9 @@
   <autoFilter ref="AP1:AS4"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Label" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="ExpRet" dataDxfId="128" totalsRowDxfId="127" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
-    <tableColumn id="3" name="Wt" totalsRowDxfId="126" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
-    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="125" totalsRowDxfId="124" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="2" name="ExpRet" dataDxfId="168" totalsRowDxfId="167" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
+    <tableColumn id="3" name="Wt" totalsRowDxfId="166" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
+    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="165" totalsRowDxfId="164" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>AQ2*AR2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9365,9 +9746,9 @@
   <autoFilter ref="AP8:AS11"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Label" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="ExpRet" dataDxfId="123" totalsRowDxfId="122" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
-    <tableColumn id="3" name="Wt" totalsRowDxfId="121" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
-    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="2" name="ExpRet" dataDxfId="163" totalsRowDxfId="162" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
+    <tableColumn id="3" name="Wt" totalsRowDxfId="161" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
+    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="160" totalsRowDxfId="159" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>AQ9*AR9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9381,8 +9762,8 @@
   <tableColumns count="9">
     <tableColumn id="1" name="Capital" dataCellStyle="Currency"/>
     <tableColumn id="2" name="Borrowed" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="LoanInt" dataDxfId="118" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Ret" dataDxfId="117" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="LoanInt" dataDxfId="158" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Ret" dataDxfId="157" dataCellStyle="Percent"/>
     <tableColumn id="5" name="TotInv">
       <calculatedColumnFormula>AU2+AV2</calculatedColumnFormula>
     </tableColumn>
@@ -9395,7 +9776,7 @@
     <tableColumn id="8" name="NetRetVal">
       <calculatedColumnFormula>AZ2-BA2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="RetRate" dataDxfId="116" dataCellStyle="Percent">
+    <tableColumn id="9" name="RetRate" dataDxfId="156" dataCellStyle="Percent">
       <calculatedColumnFormula>BB2/AU2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9407,53 +9788,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table121417" displayName="Table121417" ref="V9:AN13" totalsRowCount="1">
   <autoFilter ref="V9:AN12"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="115" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="114" totalsRowDxfId="113" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="112" totalsRowDxfId="111" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="110" totalsRowDxfId="109" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="108" totalsRowDxfId="107" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="155" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="154" totalsRowDxfId="153" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="152" totalsRowDxfId="151" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="148" totalsRowDxfId="147" dataCellStyle="Percent">
       <calculatedColumnFormula>W10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="105" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="146" totalsRowDxfId="145" dataCellStyle="Percent">
       <calculatedColumnFormula>X10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="103" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="144" totalsRowDxfId="143" dataCellStyle="Percent">
       <calculatedColumnFormula>Y10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="101" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="142" totalsRowDxfId="141" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(W10-Z$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="99" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="140" totalsRowDxfId="139" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(X10-AA$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="98" totalsRowDxfId="97" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="138" totalsRowDxfId="137" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(Y10-AB$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="96" totalsRowDxfId="95" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="136" totalsRowDxfId="135" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="94" totalsRowDxfId="93" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="134" totalsRowDxfId="133" dataCellStyle="Percent">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="92" totalsRowDxfId="91" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="132" totalsRowDxfId="131" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF10-AG10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="90" totalsRowDxfId="89" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="130" totalsRowDxfId="129" dataCellStyle="Percent">
       <calculatedColumnFormula>W10*AF$2+X10*AG$2+Y10*AH$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="88" totalsRowDxfId="87" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127" dataCellStyle="Percent">
       <calculatedColumnFormula>AI10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(AI10-AJ$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="124" totalsRowDxfId="123" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(W10-Z$13)*(X10-AA$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="122" totalsRowDxfId="121" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(W10-Z$13)*(Y10-AB$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(X10-AA$13)*(Y10-AB$13)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9465,22 +9846,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="BE1:BQ2" totalsRowShown="0">
   <autoFilter ref="BE1:BQ2"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Jret" dataDxfId="78" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="Rret" dataDxfId="77" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Jret" dataDxfId="118" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="Rret" dataDxfId="117" dataCellStyle="Percent"/>
     <tableColumn id="3" name="Jwt"/>
     <tableColumn id="4" name="Rwt">
       <calculatedColumnFormula>1-BG2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="ExpRet" dataDxfId="76" dataCellStyle="Percent">
+    <tableColumn id="5" name="ExpRet" dataDxfId="116" dataCellStyle="Percent">
       <calculatedColumnFormula>BE2*BG2+BF2*BH2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Jvol" dataDxfId="75" dataCellStyle="Percent"/>
-    <tableColumn id="7" name="Rvol" dataDxfId="74" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Jrcorr" dataDxfId="73" dataCellStyle="Comma"/>
-    <tableColumn id="9" name="Jvar" dataDxfId="72" dataCellStyle="Percent">
+    <tableColumn id="6" name="Jvol" dataDxfId="115" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Rvol" dataDxfId="114" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Jrcorr" dataDxfId="113" dataCellStyle="Comma"/>
+    <tableColumn id="9" name="Jvar" dataDxfId="112" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BJ2,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Rvar" dataDxfId="71" dataCellStyle="Percent">
+    <tableColumn id="10" name="Rvar" dataDxfId="111" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BK2,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Jrcov">
@@ -9489,7 +9870,7 @@
     <tableColumn id="12" name="Jrvar">
       <calculatedColumnFormula>BM2*BG2*BG2+BN2*BH2*BH2+2*BG2*BH2*BO2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Jrvol" dataDxfId="70" dataCellStyle="Percent">
+    <tableColumn id="13" name="Jrvol" dataDxfId="110" dataCellStyle="Percent">
       <calculatedColumnFormula>SQRT(BP2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9501,24 +9882,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1820" displayName="Table1820" ref="BE6:BQ7" totalsRowShown="0">
   <autoFilter ref="BE6:BQ7"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Jret" dataDxfId="69" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="Rret" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Jret" dataDxfId="109" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="Rret" dataDxfId="108" dataCellStyle="Percent"/>
     <tableColumn id="3" name="Jwt">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Rwt">
       <calculatedColumnFormula>1-BG7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="ExpRet" dataDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="5" name="ExpRet" dataDxfId="107" dataCellStyle="Percent">
       <calculatedColumnFormula>BE7*BG7+BF7*BH7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Jvol" dataDxfId="66" dataCellStyle="Percent"/>
-    <tableColumn id="7" name="Rvol" dataDxfId="65" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Jrcorr" dataDxfId="64" dataCellStyle="Comma"/>
-    <tableColumn id="9" name="Jvar" dataDxfId="63" dataCellStyle="Percent">
+    <tableColumn id="6" name="Jvol" dataDxfId="106" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Rvol" dataDxfId="105" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Jrcorr" dataDxfId="104" dataCellStyle="Comma"/>
+    <tableColumn id="9" name="Jvar" dataDxfId="103" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BJ7,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Rvar" dataDxfId="62" dataCellStyle="Percent">
+    <tableColumn id="10" name="Rvar" dataDxfId="102" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BK7,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Jrcov">
@@ -9527,7 +9908,7 @@
     <tableColumn id="12" name="Jrvar">
       <calculatedColumnFormula>BM7*BG7*BG7+BN7*BH7*BH7+2*BG7*BH7*BO7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Jrvol" dataDxfId="61" dataCellStyle="Percent">
+    <tableColumn id="13" name="Jrvol" dataDxfId="101" dataCellStyle="Percent">
       <calculatedColumnFormula>SQRT(BP7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9540,20 +9921,20 @@
   <autoFilter ref="F1:L6"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="311" totalsRowDxfId="310" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="309" totalsRowDxfId="308" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="351" totalsRowDxfId="350" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="349" totalsRowDxfId="348" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="307" totalsRowDxfId="306" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="347" totalsRowDxfId="346" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$2:$H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="305" totalsRowDxfId="304" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="345" totalsRowDxfId="344" dataCellStyle="Percent">
       <calculatedColumnFormula>$I2-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="303" totalsRowDxfId="302" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="343" totalsRowDxfId="342" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$2:$H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="301" totalsRowDxfId="300" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="341" totalsRowDxfId="340" dataCellStyle="Percent">
       <calculatedColumnFormula>$K2-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9566,12 +9947,12 @@
   <autoFilter ref="BS1:BW4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Security" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Ret" dataDxfId="60" totalsRowDxfId="59" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="Invested" totalsRowFunction="sum" totalsRowDxfId="58" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Wt" dataDxfId="57" totalsRowDxfId="56" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="100" totalsRowDxfId="99" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="Invested" totalsRowFunction="sum" totalsRowDxfId="98" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Wt" dataDxfId="97" totalsRowDxfId="96" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>BU2/BU$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="WtdRet" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="WtdRet" totalsRowFunction="sum" dataDxfId="95" totalsRowDxfId="94" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>BT2*BV2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9583,53 +9964,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table12141723" displayName="Table12141723" ref="V17:AN21" totalsRowCount="1">
   <autoFilter ref="V17:AN20"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="53" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="52" totalsRowDxfId="51" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="50" totalsRowDxfId="49" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="48" totalsRowDxfId="47" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="45" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="93" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="92" totalsRowDxfId="91" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="90" totalsRowDxfId="89" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="88" totalsRowDxfId="87" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Percent">
       <calculatedColumnFormula>W18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="43" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Percent">
       <calculatedColumnFormula>X18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81" dataCellStyle="Percent">
       <calculatedColumnFormula>Y18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(W18-Z$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(X18-AA$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(Y18-AB$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="74" totalsRowDxfId="73" dataCellStyle="Percent">
       <calculatedColumnFormula>0.6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="72" totalsRowDxfId="71" dataCellStyle="Percent">
       <calculatedColumnFormula>0.4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="70" totalsRowDxfId="69" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF18-AG18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="68" totalsRowDxfId="67" dataCellStyle="Percent">
       <calculatedColumnFormula>W18*AF$18+X18*AG$18+Y18*AH$18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65" dataCellStyle="Percent">
       <calculatedColumnFormula>AI18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(AI18-AJ$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(W18-Z$21)*(X18-AA$21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(W18-Z$21)*(Y18-AB$21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(X18-AA$21)*(Y18-AB$21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9654,7 +10035,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="A2:B3" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2" dataDxfId="16" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Column2" dataDxfId="56" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9665,12 +10046,12 @@
   <autoFilter ref="A4:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Investment"/>
-    <tableColumn id="2" name="Ret" dataDxfId="15" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="SD" dataDxfId="14" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Var" dataDxfId="13" dataCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="55" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="54" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="53" dataCellStyle="Comma">
       <calculatedColumnFormula>C5*C5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Utility" dataDxfId="12" dataCellStyle="Comma">
+    <tableColumn id="5" name="Utility" dataDxfId="52" dataCellStyle="Comma">
       <calculatedColumnFormula>B5-0.5*$B$2*D5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9683,12 +10064,12 @@
   <autoFilter ref="A9:E11"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Investment"/>
-    <tableColumn id="2" name="Ret" dataDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="SD" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Var" dataDxfId="9" dataCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="51" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="50" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="49" dataCellStyle="Comma">
       <calculatedColumnFormula>C10*C10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Utility" dataDxfId="8" dataCellStyle="Comma">
+    <tableColumn id="5" name="Utility" dataDxfId="48" dataCellStyle="Comma">
       <calculatedColumnFormula>B10-0.5*$B$2*D10</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9703,17 +10084,17 @@
     <tableColumn id="1" name="Investment"/>
     <tableColumn id="2" name="W1" dataCellStyle="Currency"/>
     <tableColumn id="3" name="W2" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="P1" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="5" name="P2" dataDxfId="6" dataCellStyle="Comma">
+    <tableColumn id="4" name="P1" dataDxfId="47" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="P2" dataDxfId="46" dataCellStyle="Comma">
       <calculatedColumnFormula>1-J5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="U1" dataDxfId="5">
+    <tableColumn id="6" name="U1" dataDxfId="45">
       <calculatedColumnFormula>LN(H5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="U2">
       <calculatedColumnFormula>LN(I5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="EU" dataDxfId="4">
+    <tableColumn id="8" name="EU" dataDxfId="44">
       <calculatedColumnFormula>J5*L5+K5*M5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9726,16 +10107,50 @@
   <autoFilter ref="A13:E16"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Investment"/>
-    <tableColumn id="2" name="Ret" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="SD" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Var" dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="43" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="42" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="41" dataCellStyle="Comma">
       <calculatedColumnFormula>C14*C14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Utility" dataDxfId="0" dataCellStyle="Comma">
+    <tableColumn id="5" name="Utility" dataDxfId="40" dataCellStyle="Comma">
       <calculatedColumnFormula>B14-0.5*$B$2*D14</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="ExpRet" dataDxfId="39" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="SD" dataDxfId="38" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="RiskFreeRate" dataDxfId="37" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="SharpeRatio" dataDxfId="36">
+      <calculatedColumnFormula>(A2-C2)/B2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table29" displayName="Table29" ref="F1:K4" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" headerRowCellStyle="Percent" dataCellStyle="Percent">
+  <autoFilter ref="F1:K4"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ExpExcessRet" dataDxfId="33" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="SD" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="RiskFreeRate" dataDxfId="31" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="A" dataDxfId="30" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Var" dataDxfId="29" dataCellStyle="Percent">
+      <calculatedColumnFormula>G2*G2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="w" dataDxfId="28" dataCellStyle="Percent">
+      <calculatedColumnFormula>F2/(I2*J2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -9747,14 +10162,125 @@
     <tableColumn id="2" name="Probability" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
     <tableColumn id="3" name="YrEndPrice" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
     <tableColumn id="4" name="CashFlow" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="299" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="5" name="Ret" dataDxfId="339" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>($P2+$Q2)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="298" totalsRowDxfId="297" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="338" totalsRowDxfId="337" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O2*$R2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table30" displayName="Table30" ref="M1:P2" totalsRowShown="0">
+  <autoFilter ref="M1:P2"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="RiskyRet" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="RiskFreeRet" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="TargetRet" dataDxfId="25" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="wRisky" dataDxfId="24" dataCellStyle="Comma">
+      <calculatedColumnFormula>(O2-N2)/(M2-N2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table31" displayName="Table31" ref="R1:T3" totalsRowShown="0">
+  <autoFilter ref="R1:T3"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="RiskySD" dataDxfId="23" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="TargetSD" dataDxfId="22" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="wRisky" dataDxfId="21" dataCellStyle="Percent">
+      <calculatedColumnFormula>S2/R2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Table32" displayName="Table32" ref="V1:AA2" totalsRowShown="0">
+  <autoFilter ref="V1:AA2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="riskySD" dataDxfId="20" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="riskyRet" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="riskFreeRet" dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="targSD" dataDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="riskyWt" dataDxfId="16" dataCellStyle="Comma">
+      <calculatedColumnFormula>Y2/V2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="pfRet" dataDxfId="15" dataCellStyle="Percent">
+      <calculatedColumnFormula>Z2*W2+(1-Z2)*X2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Table33" displayName="Table33" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="DivInv" dataDxfId="14" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="FelixInv" dataDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Total" dataDxfId="12" dataCellStyle="Currency">
+      <calculatedColumnFormula>A2+B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="DivWt" dataDxfId="11" dataCellStyle="Comma">
+      <calculatedColumnFormula>A2/C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="FelixWt" dataDxfId="10" dataCellStyle="Comma">
+      <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="TotWt" dataDxfId="9" dataCellStyle="Comma">
+      <calculatedColumnFormula>D2+E2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="Table34" displayName="Table34" ref="H1:K3" totalsRowShown="0">
+  <autoFilter ref="H1:K3"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Desc"/>
+    <tableColumn id="2" name="Ret" dataDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="3" dataCellStyle="Comma">
+      <calculatedColumnFormula>J2*J2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="Table35" displayName="Table35" ref="M1:M2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowCellStyle="Percent" dataCellStyle="Percent">
+  <autoFilter ref="M1:M2"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="pfRet" dataDxfId="7" dataCellStyle="Percent">
+      <calculatedColumnFormula>D2*I2+E2*I3</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="Table36" displayName="Table36" ref="O1:P2" totalsRowShown="0" dataDxfId="0" dataCellStyle="Comma">
+  <autoFilter ref="O1:P2"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Corr" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Cov" dataDxfId="1" dataCellStyle="Comma">
+      <calculatedColumnFormula>O2*J2*J3</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -9763,20 +10289,20 @@
   <autoFilter ref="F9:L12"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="296" totalsRowDxfId="295" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="294" totalsRowDxfId="293" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="336" totalsRowDxfId="335" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="334" totalsRowDxfId="333" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="292" totalsRowDxfId="291" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="332" totalsRowDxfId="331" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$10:$H10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="290" totalsRowDxfId="289" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="330" totalsRowDxfId="329" dataCellStyle="Percent">
       <calculatedColumnFormula>$I10-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="288" totalsRowDxfId="287" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="328" totalsRowDxfId="327" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$10:$H10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="286" totalsRowDxfId="285" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="326" totalsRowDxfId="325" dataCellStyle="Percent">
       <calculatedColumnFormula>$K10-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9788,22 +10314,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="O9:V13" totalsRowCount="1">
   <autoFilter ref="O9:V12"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="284" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="283" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="282" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="281" totalsRowDxfId="280" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="324" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="323" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="322" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="321" totalsRowDxfId="320" dataCellStyle="Percent">
       <calculatedColumnFormula>($P10+$Q10)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="319" totalsRowDxfId="318" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O10*$R10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="317" totalsRowDxfId="316" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R10-$S$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="315" totalsRowDxfId="314" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T10*$O10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="273" totalsRowDxfId="272" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="313" totalsRowDxfId="312" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U13)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9815,22 +10341,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table378" displayName="Table378" ref="O16:V20" totalsRowCount="1">
   <autoFilter ref="O16:V19"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="271" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="270" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="269" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="268" totalsRowDxfId="267" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="311" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="310" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="309" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="308" totalsRowDxfId="307" dataCellStyle="Percent">
       <calculatedColumnFormula>($P17+$Q17)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="266" totalsRowDxfId="265" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="306" totalsRowDxfId="305" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O17*$R17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="264" totalsRowDxfId="263" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="304" totalsRowDxfId="303" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R17-$S$20,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="262" totalsRowDxfId="261" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="302" totalsRowDxfId="301" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T17*$O17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="260" totalsRowDxfId="259" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="300" totalsRowDxfId="299" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U20)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9843,20 +10369,20 @@
   <autoFilter ref="F15:L18"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="258" totalsRowDxfId="257" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="256" totalsRowDxfId="255" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="298" totalsRowDxfId="297" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="296" totalsRowDxfId="295" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G16</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="254" totalsRowDxfId="253" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="294" totalsRowDxfId="293" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$16:$H16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="252" totalsRowDxfId="251" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="292" totalsRowDxfId="291" dataCellStyle="Percent">
       <calculatedColumnFormula>$I16-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="250" totalsRowDxfId="249" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="290" totalsRowDxfId="289" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$16:$H16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="248" totalsRowDxfId="247" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="288" totalsRowDxfId="287" dataCellStyle="Percent">
       <calculatedColumnFormula>$K16-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9868,22 +10394,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table3789" displayName="Table3789" ref="O23:V27" totalsRowCount="1">
   <autoFilter ref="O23:V26"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="246" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="245" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="244" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="243" totalsRowDxfId="242" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="286" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="285" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="284" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="283" totalsRowDxfId="282" dataCellStyle="Percent">
       <calculatedColumnFormula>($P24+$Q24)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="241" totalsRowDxfId="240" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="281" totalsRowDxfId="280" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O24*$R24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="239" totalsRowDxfId="238" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R24-$S$27,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="237" totalsRowDxfId="236" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T24*$O24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="235" totalsRowDxfId="234" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U27)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9896,20 +10422,20 @@
   <autoFilter ref="F23:L28"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="233" totalsRowDxfId="232" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="231" totalsRowDxfId="230" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="273" totalsRowDxfId="272" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="271" totalsRowDxfId="270" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="229" totalsRowDxfId="228" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="269" totalsRowDxfId="268" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$24:$H24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="227" totalsRowDxfId="226" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="267" totalsRowDxfId="266" dataCellStyle="Percent">
       <calculatedColumnFormula>$I24-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="225" totalsRowDxfId="224" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="265" totalsRowDxfId="264" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$24:$H24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="223" totalsRowDxfId="222" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="263" totalsRowDxfId="262" dataCellStyle="Percent">
       <calculatedColumnFormula>$K24-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11564,6 +12090,267 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="34"/>
+    <col min="5" max="5" width="9.36328125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="34"/>
+    <col min="9" max="10" width="8.7265625" style="2"/>
+    <col min="11" max="11" width="8.7265625" style="34"/>
+    <col min="13" max="14" width="8.7265625" style="12"/>
+    <col min="15" max="15" width="8.7265625" style="36"/>
+    <col min="16" max="16" width="8.7265625" style="34"/>
+    <col min="38" max="38" width="8.7265625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A2" s="37">
+        <v>600000</v>
+      </c>
+      <c r="B2" s="37">
+        <v>100000</v>
+      </c>
+      <c r="C2" s="37">
+        <f>A2+B2</f>
+        <v>700000</v>
+      </c>
+      <c r="D2" s="34">
+        <f>A2/C2</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="E2" s="34">
+        <f>B2/C2</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F2" s="34">
+        <f>D2+E2</f>
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K2" s="34">
+        <f t="shared" ref="K2:K3" si="0">J2*J2</f>
+        <v>7.8400000000000011E-2</v>
+      </c>
+      <c r="M2" s="12">
+        <f>D2*I2+E2*I3</f>
+        <v>0.09</v>
+      </c>
+      <c r="O2" s="36">
+        <v>0.4</v>
+      </c>
+      <c r="P2" s="34">
+        <f>O2*J2*J3</f>
+        <v>3.9200000000000006E-2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>158</v>
+      </c>
+      <c r="S2" t="s">
+        <v>159</v>
+      </c>
+      <c r="V2" t="s">
+        <v>158</v>
+      </c>
+      <c r="W2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="K3" s="34">
+        <f t="shared" si="0"/>
+        <v>0.12249999999999998</v>
+      </c>
+      <c r="R3" s="24">
+        <f>D2</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="S3" s="24">
+        <f>E2</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="U3" t="s">
+        <v>158</v>
+      </c>
+      <c r="V3" s="24">
+        <f>K2</f>
+        <v>7.8400000000000011E-2</v>
+      </c>
+      <c r="W3" s="24">
+        <f>$P$2</f>
+        <v>3.9200000000000006E-2</v>
+      </c>
+      <c r="Y3">
+        <f t="array" ref="Y3:Z3">MMULT(R3:S3,V3:W4)</f>
+        <v>7.2800000000000004E-2</v>
+      </c>
+      <c r="Z3">
+        <v>5.1100000000000007E-2</v>
+      </c>
+      <c r="AB3">
+        <f t="array" ref="AB3:AB4">TRANSPOSE(R3:S3)</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="AD3">
+        <f>MMULT(Y3:Z3,AB3:AB4)</f>
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="AE3" s="2">
+        <f>SQRT(AD3)</f>
+        <v>0.26400757564888172</v>
+      </c>
+      <c r="AG3">
+        <v>0.08</v>
+      </c>
+      <c r="AH3">
+        <v>0.05</v>
+      </c>
+      <c r="AI3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AJ3">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="AK3">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AL3" s="15">
+        <f>SUMPRODUCT(AG3:AH3,AJ3:AK3)</f>
+        <v>7.571428571428572E-2</v>
+      </c>
+      <c r="AM3">
+        <f>AI3*AJ3</f>
+        <v>0.24000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="U4" t="s">
+        <v>159</v>
+      </c>
+      <c r="V4" s="24">
+        <f>$P$2</f>
+        <v>3.9200000000000006E-2</v>
+      </c>
+      <c r="W4" s="24">
+        <f>K3</f>
+        <v>0.12249999999999998</v>
+      </c>
+      <c r="AB4">
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW22"/>
@@ -23974,7 +24761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -24294,4 +25081,265 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA4"/>
+  <sheetViews>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="2"/>
+    <col min="8" max="8" width="14.36328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="24"/>
+    <col min="13" max="13" width="10.36328125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.36328125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" style="34"/>
+    <col min="18" max="18" width="9.36328125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10.36328125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8.7265625" style="2"/>
+    <col min="22" max="22" width="9.36328125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="10.36328125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="13.36328125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="8.7265625" style="2"/>
+    <col min="26" max="26" width="9.36328125" style="34" customWidth="1"/>
+    <col min="27" max="27" width="9.54296875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z1" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="C2" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D2" s="24">
+        <f>(A2-C2)/B2</f>
+        <v>0.34374999999999994</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="I2" s="35">
+        <v>4</v>
+      </c>
+      <c r="J2" s="25">
+        <f>G2*G2</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="K2" s="2">
+        <f>F2/(I2*J2)</f>
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="N2" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="P2" s="34">
+        <f>(O2-N2)/(M2-N2)</f>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="T2" s="2">
+        <f>S2/R2</f>
+        <v>1.40625</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="Z2" s="34">
+        <f>Y2/V2</f>
+        <v>0.8</v>
+      </c>
+      <c r="AA2" s="2">
+        <f>Z2*W2+(1-Z2)*X2</f>
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D3" s="24">
+        <f>(A3-C3)/B3</f>
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I3" s="35">
+        <v>3</v>
+      </c>
+      <c r="J3" s="25">
+        <f>G3*G3</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <f>F3/(I3*J3)</f>
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="T3" s="2">
+        <f>S3/R3</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>8.1920692799618278E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="I4" s="35">
+        <v>4</v>
+      </c>
+      <c r="J4" s="25">
+        <f>G4*G4</f>
+        <v>6.71099990876943E-3</v>
+      </c>
+      <c r="K4" s="2">
+        <f>F4/(I4*J4)</f>
+        <v>1.7732081898034264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Portfolio risk week 5.
</commit_message>
<xml_diff>
--- a/ClassesTaken/Coursera/2016/InvManagementRice/02PortfolioRisk/PortfolioRisk.xlsx
+++ b/ClassesTaken/Coursera/2016/InvManagementRice/02PortfolioRisk/PortfolioRisk.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14928" windowHeight="8076" tabRatio="702" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14928" windowHeight="8076" tabRatio="702" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="wk01" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="wk03" sheetId="8" r:id="rId8"/>
     <sheet name="wk04" sheetId="9" r:id="rId9"/>
     <sheet name="Felix" sheetId="10" r:id="rId10"/>
+    <sheet name="wk05" sheetId="11" r:id="rId11"/>
+    <sheet name="FamaFrench" sheetId="12" r:id="rId12"/>
+    <sheet name="quiz05" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="229">
   <si>
     <t>P0</t>
   </si>
@@ -560,12 +563,189 @@
   <si>
     <t>PfSD</t>
   </si>
+  <si>
+    <t>RisklessRate</t>
+  </si>
+  <si>
+    <t>RiskyRate</t>
+  </si>
+  <si>
+    <t>RiskyVol</t>
+  </si>
+  <si>
+    <t>RiskyPortion</t>
+  </si>
+  <si>
+    <t>ExcessRate</t>
+  </si>
+  <si>
+    <t>RiskyVar</t>
+  </si>
+  <si>
+    <t>AveGamma</t>
+  </si>
+  <si>
+    <t>MktPfRet</t>
+  </si>
+  <si>
+    <t>MktPfVar</t>
+  </si>
+  <si>
+    <t>VarZ</t>
+  </si>
+  <si>
+    <t>CorrMktZ</t>
+  </si>
+  <si>
+    <t>VolMkt</t>
+  </si>
+  <si>
+    <t>VolZ</t>
+  </si>
+  <si>
+    <t>MktExcessRet</t>
+  </si>
+  <si>
+    <t>BetaZ</t>
+  </si>
+  <si>
+    <t>Zret</t>
+  </si>
+  <si>
+    <t>MktPfVol</t>
+  </si>
+  <si>
+    <t>TargRet</t>
+  </si>
+  <si>
+    <t>TargVol</t>
+  </si>
+  <si>
+    <t>TargExcessRet</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>MktRate</t>
+  </si>
+  <si>
+    <t>MktExcessRate</t>
+  </si>
+  <si>
+    <t>BetaWtdAve</t>
+  </si>
+  <si>
+    <t>RetWtdAve</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Aprice</t>
+  </si>
+  <si>
+    <t>VarSub</t>
+  </si>
+  <si>
+    <t>MktRet</t>
+  </si>
+  <si>
+    <t>MktVol</t>
+  </si>
+  <si>
+    <t>StockVol</t>
+  </si>
+  <si>
+    <t>StockBeta</t>
+  </si>
+  <si>
+    <t>RisklessRet</t>
+  </si>
+  <si>
+    <t>StockExcessRet</t>
+  </si>
+  <si>
+    <t>StockRet</t>
+  </si>
+  <si>
+    <t>Bmkt</t>
+  </si>
+  <si>
+    <t>Bsmb</t>
+  </si>
+  <si>
+    <t>Bhml</t>
+  </si>
+  <si>
+    <t>Mkt-rf</t>
+  </si>
+  <si>
+    <t>SMB</t>
+  </si>
+  <si>
+    <t>HML</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t>MonthlyRet</t>
+  </si>
+  <si>
+    <t>YrlyRet</t>
+  </si>
+  <si>
+    <t>Despression</t>
+  </si>
+  <si>
+    <t>Bprice</t>
+  </si>
+  <si>
+    <t>vol_A</t>
+  </si>
+  <si>
+    <t>vol_B</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>corr</t>
+  </si>
+  <si>
+    <t>CorrMktA</t>
+  </si>
+  <si>
+    <t>CorrMktB</t>
+  </si>
+  <si>
+    <t>CovMktA</t>
+  </si>
+  <si>
+    <t>CovMktB</t>
+  </si>
+  <si>
+    <t>CovMktPf</t>
+  </si>
+  <si>
+    <t>CorrMktPf</t>
+  </si>
+  <si>
+    <t>BetaPf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="12">
+  <numFmts count="13">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -576,8 +756,9 @@
     <numFmt numFmtId="169" formatCode="0.000000"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="0.00000%"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
-    <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="173" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -658,7 +839,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
@@ -695,8 +876,10 @@
     <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -704,7 +887,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="353">
+  <dxfs count="428">
     <dxf>
       <font>
         <b val="0"/>
@@ -722,6 +905,235 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="167" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="174" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="174" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -743,6 +1155,9 @@
       <numFmt numFmtId="170" formatCode="0.0000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -759,7 +1174,278 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="173" formatCode="0.000"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="174" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -781,18 +1467,74 @@
       <numFmt numFmtId="170" formatCode="0.0000"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="172" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.000%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000%"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
@@ -805,13 +1547,13 @@
       <numFmt numFmtId="170" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="173" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -4610,7 +5352,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5546DD3E-6C38-4588-BC37-7394D37D3BB9}" type="CELLRANGE">
+                    <a:fld id="{1A15EC63-8464-4C4D-BF1B-ECD527F6C379}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4643,7 +5385,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F550AC5-ED97-4A3C-82BB-CBBDD1A15E8A}" type="CELLRANGE">
+                    <a:fld id="{190D1918-C5E9-4693-8B6E-C341449FB55E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4676,7 +5418,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E469D964-7C07-458C-944B-143E31EB9C20}" type="CELLRANGE">
+                    <a:fld id="{B9488F7D-A6E6-401C-8787-4C6595B38B0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4709,7 +5451,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0239713-D04C-47A9-8937-BD9B479F5A62}" type="CELLRANGE">
+                    <a:fld id="{40B49433-7E42-4CD9-951E-85AA36D3E9F4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4742,7 +5484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5FE7718F-7923-41A4-A39A-79130B55D7C2}" type="CELLRANGE">
+                    <a:fld id="{C546EC35-536B-4551-A6C6-F0D95BDE6944}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4775,7 +5517,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0634DD1D-CDD0-4C5A-99FF-7AAC238C69A3}" type="CELLRANGE">
+                    <a:fld id="{A91EBC5A-26EB-4655-9A2E-B4D277DD1477}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4808,7 +5550,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B86A0263-2A9B-43A7-A2AF-6774B48374A8}" type="CELLRANGE">
+                    <a:fld id="{C817229D-70F7-4F8D-8440-DA954C8B6E15}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4841,7 +5583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5F8506E-6D4D-41F7-9DAD-AC0CF962AE88}" type="CELLRANGE">
+                    <a:fld id="{1A69F049-10AB-4286-8D8B-BA4863AA7C73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4874,7 +5616,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBEB418D-7E5F-415F-8487-89721300A9DC}" type="CELLRANGE">
+                    <a:fld id="{01D4713F-8BC4-4B31-97F0-979FE919D490}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4907,7 +5649,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92CDFA4F-D3CF-4F25-B786-D636DDEA1754}" type="CELLRANGE">
+                    <a:fld id="{5C7D871B-2443-4DD8-A0B5-21B8D5F5D931}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4940,7 +5682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94269597-8AA6-4598-A1A8-BB6F4A355220}" type="CELLRANGE">
+                    <a:fld id="{292145B3-AB58-4B85-9706-68F46DEE4A9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4973,7 +5715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{224CFF0C-FB32-4206-AC91-18C503CC4C0C}" type="CELLRANGE">
+                    <a:fld id="{CFF2A8CF-5EB1-461C-AA42-05D21B188C0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5006,7 +5748,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8ACF232-282A-422E-8651-9D789547E117}" type="CELLRANGE">
+                    <a:fld id="{7A20F4FC-0FF8-4C06-8B11-59B0A69EB904}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5039,7 +5781,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5EDD2AD-68CD-4FE2-9072-2DC399E195AD}" type="CELLRANGE">
+                    <a:fld id="{0FA5F501-64F2-4D26-BB43-12B061A2AAF4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5072,7 +5814,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{725B8A45-3341-4C0B-9490-01B87C76689A}" type="CELLRANGE">
+                    <a:fld id="{63282687-B019-4FFA-B7E0-BA217A64D4A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5105,7 +5847,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B84BC46-FCDA-4A0A-B4FB-4755FDAF9A2C}" type="CELLRANGE">
+                    <a:fld id="{FE976668-CB8C-4E82-9C25-C819DC520EF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5138,7 +5880,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E00DB2C8-6778-464E-9363-4BFE8281E5BE}" type="CELLRANGE">
+                    <a:fld id="{78E52AC6-AA58-4C2B-BF4B-DDF293DC5657}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5171,7 +5913,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7ABCEC7C-712D-4325-9EE2-A64177D8BE8C}" type="CELLRANGE">
+                    <a:fld id="{A721888D-F76A-4EA2-B4B7-C4505A4E6D45}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5204,7 +5946,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB59660D-C0E9-40AF-9CB7-256035B2F10C}" type="CELLRANGE">
+                    <a:fld id="{0C8CD435-AC55-4653-B02A-A14773FF1E30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5237,7 +5979,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BDC5895-F53B-4592-AA54-1D20900C06CA}" type="CELLRANGE">
+                    <a:fld id="{E870F91C-1B39-432E-9CB0-5068231A80EA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5270,7 +6012,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{982D65CF-4292-4AE3-AB32-150DF73A8F02}" type="CELLRANGE">
+                    <a:fld id="{B105A668-1ADE-49AC-A76D-B4327BB8C2D0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5303,7 +6045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE9B8273-C2A8-4EE0-9B41-60352A5B7AB8}" type="CELLRANGE">
+                    <a:fld id="{1C606FD1-DD34-4E9F-AA57-79966AA577E6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5336,7 +6078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{471D99AE-A4B5-407B-A7A1-4E65A4F0FA30}" type="CELLRANGE">
+                    <a:fld id="{AB622C03-390B-4323-87C8-3C88DA26E4CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5369,7 +6111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5258CF8A-CD79-4410-A9EC-A8A86F3B7D36}" type="CELLRANGE">
+                    <a:fld id="{52DA9F9F-A631-4DD9-A80C-6A8F0417515E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5402,7 +6144,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3C3E9BE3-415D-41A6-968E-ABF8B674BF2A}" type="CELLRANGE">
+                    <a:fld id="{BA1C764A-C4CB-4993-BF37-04AB0AF16039}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5435,7 +6177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A18004C3-4763-4F2C-8AF9-3F431DAFFB86}" type="CELLRANGE">
+                    <a:fld id="{05EE34FA-F4F6-4B6A-BF7C-21CAB854F337}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5468,7 +6210,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B851863A-1C76-4218-8511-6D75C5DDD04E}" type="CELLRANGE">
+                    <a:fld id="{72DDE15A-5077-4888-8F3A-9B71FC4424FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5501,7 +6243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B10E785F-836E-4973-9851-69755D9EC970}" type="CELLRANGE">
+                    <a:fld id="{9E9AA386-C637-4ED4-84F6-B46A8298FD4A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5534,7 +6276,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5DB148C-6FD6-492F-926E-A807B66ED9A8}" type="CELLRANGE">
+                    <a:fld id="{61A896BE-E0C4-4578-9F79-7E1F63E41DA4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5567,7 +6309,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF892B70-19F8-40CD-AF54-42BFBCAD4F5A}" type="CELLRANGE">
+                    <a:fld id="{24432FBF-206A-4C32-B43E-73D8CA16321C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5600,7 +6342,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2662B45F-FDB5-4077-AEFA-A4C20E7BBF19}" type="CELLRANGE">
+                    <a:fld id="{9B5FB8F1-818E-4907-BDB7-FC19B44E5E2B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5633,7 +6375,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9803C19-D934-4BDD-AF92-D038EFE11B0B}" type="CELLRANGE">
+                    <a:fld id="{39669A39-09EC-43D6-B795-32438AB79853}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5666,7 +6408,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B5F7519-2D4A-4F81-977F-629BFAA1DF8F}" type="CELLRANGE">
+                    <a:fld id="{94AE4519-5471-449E-8336-1FD462520821}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5699,7 +6441,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13DE5BA7-24AF-479F-ADD7-D580CBCF23E8}" type="CELLRANGE">
+                    <a:fld id="{C820C6D9-F073-459B-9032-B014D9C5E1CB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5732,7 +6474,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86A922EC-BE03-4DDD-832B-56BA766A74E4}" type="CELLRANGE">
+                    <a:fld id="{3C940C90-CD7D-4514-A9A7-1401E45AC457}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5765,7 +6507,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFB47D17-5EEF-4987-BB11-36913091F9FF}" type="CELLRANGE">
+                    <a:fld id="{707BE580-F31A-4100-B7C8-C6DD8894BA8B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5798,7 +6540,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{849B78C2-D93C-4225-8097-C04C8C3950BE}" type="CELLRANGE">
+                    <a:fld id="{748DF55D-10BB-4D6A-9C14-2D4DA7E0D941}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5831,7 +6573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14FD3B05-3183-48B4-8656-0E26579BA802}" type="CELLRANGE">
+                    <a:fld id="{9BEDC807-8201-49FE-8F69-D46F29B57A20}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5864,7 +6606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0B301E80-A101-415E-A9C7-F7D0EB6B0823}" type="CELLRANGE">
+                    <a:fld id="{E5492E24-DDD0-4712-AEB0-941B73955282}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5897,7 +6639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC159138-0EDA-41AB-A95B-583B794C9EFE}" type="CELLRANGE">
+                    <a:fld id="{3CA68693-6F96-44E4-BF57-B1B7774C17AF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5930,7 +6672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB551726-75AF-425B-8960-B189C8FF3FAE}" type="CELLRANGE">
+                    <a:fld id="{FE048DF6-AFB6-4C93-8656-E4937249BEC8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5963,7 +6705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02C38043-120D-426B-8833-2B48DD219129}" type="CELLRANGE">
+                    <a:fld id="{7AEE8E01-4695-4742-8C8E-3597B575BB17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5996,7 +6738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC697B59-A13B-49CE-8EC4-1B078B03A1AD}" type="CELLRANGE">
+                    <a:fld id="{1C8A81AE-CBE8-4CF8-9DF8-4D3092960D0A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6029,7 +6771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD33B331-044E-4DEC-9135-0CCCFC2EEFE9}" type="CELLRANGE">
+                    <a:fld id="{E3EDEE1E-D944-43B7-8DFC-02A7240884DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6062,7 +6804,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2071E286-9B08-4BE6-B735-2B39545DCB4F}" type="CELLRANGE">
+                    <a:fld id="{C2ABA9EE-7C81-4F7D-8D20-78CA9BCC9EE3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6095,7 +6837,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF9000AA-D817-4682-85ED-27928F44D021}" type="CELLRANGE">
+                    <a:fld id="{3C737035-8F21-404D-BDFF-E2A017C811CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6128,7 +6870,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23150F83-8A76-442F-B288-03F9841E8219}" type="CELLRANGE">
+                    <a:fld id="{DA67CA5D-9122-4E9F-9867-010B98011BBA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6161,7 +6903,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5B0B3A1-AC06-4C1F-BDA8-84308A1B6901}" type="CELLRANGE">
+                    <a:fld id="{BD168D37-AB75-42B9-A282-B48C206930A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6194,7 +6936,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFD6BFB0-DC42-48E0-BD8D-D201E621B3E8}" type="CELLRANGE">
+                    <a:fld id="{FB6884CC-5A3C-4409-AA8E-8B66A6300D99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6227,7 +6969,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE74049C-6365-4578-A979-137C89BC25E5}" type="CELLRANGE">
+                    <a:fld id="{F734C418-ACEE-4DA8-82F7-AADF39B5D55C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6260,7 +7002,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{319B60DB-4495-4981-959E-ACF78C754C47}" type="CELLRANGE">
+                    <a:fld id="{AE544464-78AC-44C3-87CB-77DDD378B1AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6293,7 +7035,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{16C070FF-F401-4D7F-8E4A-2ECED647E329}" type="CELLRANGE">
+                    <a:fld id="{7B2258B4-A7DD-409C-A409-05E702504400}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6326,7 +7068,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34BFC6B0-A5C6-42D4-A369-315FE5188427}" type="CELLRANGE">
+                    <a:fld id="{F361BCA5-41EC-4AB2-B67B-D1B0D8AB42A6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6359,7 +7101,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DAF444B0-7668-42FE-B392-C92C3E77EB76}" type="CELLRANGE">
+                    <a:fld id="{312D9B88-67A8-4998-8943-CF8C0FBC5516}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6392,7 +7134,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F67A0D88-F5A0-4174-A9D5-2FDF3A58A7E4}" type="CELLRANGE">
+                    <a:fld id="{656E7D92-C67B-46AF-A762-1C57CF7DA4CF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6425,7 +7167,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{599B789E-E7E1-484B-80A3-2F67ACF5D5AD}" type="CELLRANGE">
+                    <a:fld id="{F3C67471-513A-4F14-80BE-289B4B77AF95}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6458,7 +7200,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7A8FDE4-D3F5-4A32-A0E7-7F8E4C66C692}" type="CELLRANGE">
+                    <a:fld id="{1EF92E64-7306-4BD4-9C4F-3D6CA445A62A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6491,7 +7233,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CBB1A62-1848-4422-8F08-C88B04B50BD1}" type="CELLRANGE">
+                    <a:fld id="{9F29477C-CC6D-43A0-8496-39AE066F4567}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6524,7 +7266,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD196D26-BF39-4F37-A722-3C8B73D89F3B}" type="CELLRANGE">
+                    <a:fld id="{5CA9DDBE-06BE-4FDF-8554-6EBDB55CA30C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6557,7 +7299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF562CAF-0615-4AFA-A9AC-D794A93A0E92}" type="CELLRANGE">
+                    <a:fld id="{4998C840-D998-40D7-836A-0772907BF8B7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6590,7 +7332,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86F521B4-C975-47F2-B001-6C29C41839E8}" type="CELLRANGE">
+                    <a:fld id="{BA2FCF1B-2E8E-4510-B259-3D5C2AFDF234}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6623,7 +7365,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6D93F50-D0AB-4845-B2F4-5A41BCA4780C}" type="CELLRANGE">
+                    <a:fld id="{17745B3D-7715-41EE-9A59-C874BE06075B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6656,7 +7398,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A14C5AB-62A0-4302-88C0-AAFFF5A4D9F0}" type="CELLRANGE">
+                    <a:fld id="{D4BFB579-F207-4E76-886E-53F2EB008C1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6689,7 +7431,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8C95B39-3F4C-45EA-9AAF-1D30C6DCBBD8}" type="CELLRANGE">
+                    <a:fld id="{93330495-5B52-4B74-A11B-5F70F538CB70}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6722,7 +7464,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F0ABDE2-5FA1-456F-A76C-31B77AC2DA72}" type="CELLRANGE">
+                    <a:fld id="{303D4471-98B3-4B78-8FD7-335ACFE59DA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6755,7 +7497,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40728121-34E1-4ECB-B2DD-15461F552AA5}" type="CELLRANGE">
+                    <a:fld id="{67DFA4E3-9795-4FF6-AD34-54691929271D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6788,7 +7530,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3463F136-4702-408B-9C3C-404EB2C6389D}" type="CELLRANGE">
+                    <a:fld id="{3299A456-9493-4A1D-BDB7-48DC35A93A48}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6821,7 +7563,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60217F84-6FB4-43F9-9D7E-008993D9EE59}" type="CELLRANGE">
+                    <a:fld id="{1EC8128A-A98F-44DA-AA6D-C83F58CF5F7C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6854,7 +7596,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12587F89-4787-40CE-9C2A-FB16455AF63D}" type="CELLRANGE">
+                    <a:fld id="{232184E9-897E-41B0-83CB-662A1864498E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6887,7 +7629,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36C61D10-5241-421B-8946-B796B2BDE709}" type="CELLRANGE">
+                    <a:fld id="{CD7BB29C-E0F7-4EFD-8176-65BA43A5F197}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6920,7 +7662,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{135C79AF-F7ED-4EE6-8630-A538D6279F88}" type="CELLRANGE">
+                    <a:fld id="{AB78AAF8-F278-4104-9D9C-90169765AA6E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6953,7 +7695,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C9520DB-8BC7-4590-A9E8-57DABFF1AB05}" type="CELLRANGE">
+                    <a:fld id="{96303C69-BE66-471C-9E8B-677B95A5D7BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6986,7 +7728,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58173E57-200F-4E54-AF12-EE6592436E99}" type="CELLRANGE">
+                    <a:fld id="{B6371D1B-B2FE-458D-A166-A68C0ABDCB37}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7019,7 +7761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59A55068-7B23-4A79-8156-23EC562B7A5C}" type="CELLRANGE">
+                    <a:fld id="{6045F2E7-3EC7-469C-8010-6DD284BA79AD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7052,7 +7794,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7403EF6-64A9-410E-B1E2-37EB587C193D}" type="CELLRANGE">
+                    <a:fld id="{B9277955-32C9-4B64-9D55-F02742E78106}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7085,7 +7827,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB663849-4653-41E1-AD8B-E2DCCF4B4D67}" type="CELLRANGE">
+                    <a:fld id="{BE3E2CF0-4D8E-4358-B57D-40C0E04B5C37}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7118,7 +7860,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3EA022C-8BE3-4D47-8BF6-582FD3B2B85A}" type="CELLRANGE">
+                    <a:fld id="{7A5A8F39-A284-4858-B403-5EED68617B3E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7151,7 +7893,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CAF838E-881A-4926-8632-C7928F818505}" type="CELLRANGE">
+                    <a:fld id="{3E313E17-0322-4E6F-B923-987AA8B182C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7184,7 +7926,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC3B0EA7-E9BB-4246-A670-EC2DC8230C03}" type="CELLRANGE">
+                    <a:fld id="{AF067C39-594D-4F61-8E14-16503D777A83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7217,7 +7959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{582A26FE-7D19-46A6-8AEC-3B07CEAB8D99}" type="CELLRANGE">
+                    <a:fld id="{389C3A15-68C1-4E43-B797-DAFACD6D0BBA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7250,7 +7992,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CEE8AB5-5F39-41B4-B4AD-44C2771B37A8}" type="CELLRANGE">
+                    <a:fld id="{AAC444BB-7ED0-4077-95E5-F019770474F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7283,7 +8025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19D6A829-DA3D-478A-8EC7-03FDFFE4FE4E}" type="CELLRANGE">
+                    <a:fld id="{16BE9354-AB2D-49F0-82B0-5457665C2B22}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7316,7 +8058,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CD9AD94-227E-473A-A556-11427797C00D}" type="CELLRANGE">
+                    <a:fld id="{62BF548E-9A18-4942-A700-144D4025E60E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7349,7 +8091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E143CD50-B47B-40CD-AECF-8B6D14153590}" type="CELLRANGE">
+                    <a:fld id="{1E6869D0-A4D8-466D-8B63-E796AB790798}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7382,7 +8124,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A23CEAB5-62FE-449E-B198-BEC8213A64D9}" type="CELLRANGE">
+                    <a:fld id="{6283C9C4-704B-48E0-9258-7577CB9EF1D9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7415,7 +8157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{14B8C6E1-7D34-42A9-A94D-9D3BB9FFC5D0}" type="CELLRANGE">
+                    <a:fld id="{038DA88B-8794-4D1F-B396-49D1CA262EDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7448,7 +8190,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F7B7C73E-A02C-4177-848D-52E30E2E31D2}" type="CELLRANGE">
+                    <a:fld id="{E1C89CF7-38CB-4842-A7D4-B3FBAFC492EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7481,7 +8223,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5C501B8-164A-4F18-8E0F-6E5C31F196EF}" type="CELLRANGE">
+                    <a:fld id="{22FF4CF5-D047-4E43-827A-9EC5FFE0F401}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7514,7 +8256,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8847FB3-64CA-49AA-99FA-AF994A9210CF}" type="CELLRANGE">
+                    <a:fld id="{9C2E4AE0-48B2-43F5-BE92-AD06EE049E89}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7547,7 +8289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6BB4EDD9-8C50-4C72-AA44-5D9F17580F88}" type="CELLRANGE">
+                    <a:fld id="{113945F0-8946-468E-B684-929DCC4C5B90}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7580,7 +8322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{361FE5B0-19F2-4857-B02D-F69C687AB13B}" type="CELLRANGE">
+                    <a:fld id="{17D44A13-FBE9-407A-8536-A5C5CF30CB61}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7613,7 +8355,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D3E5009-7F4F-4CFC-8906-2137E3CC5937}" type="CELLRANGE">
+                    <a:fld id="{729FE14A-8A1D-4532-8F71-9318A3560343}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7646,7 +8388,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D906CB0A-1F33-4239-984D-2EF36013D3DA}" type="CELLRANGE">
+                    <a:fld id="{058E7443-AA94-45AD-92DA-47959CF0E631}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7679,7 +8421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{98D1921D-19CE-45DC-8CA8-F083869FE7F8}" type="CELLRANGE">
+                    <a:fld id="{7F0F5146-627F-4EAD-A064-D5DD3AD3331B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7712,7 +8454,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39B36489-8B10-441B-99F5-B139A6261B86}" type="CELLRANGE">
+                    <a:fld id="{6FFDAC8F-5417-49E3-A499-A5DC0AA24D91}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7745,7 +8487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A7365C9-FC21-4310-8A59-E223CC18567A}" type="CELLRANGE">
+                    <a:fld id="{8D868095-6B6F-4638-AE73-0B047EBAA2BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7778,7 +8520,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FE51C8B-D905-4213-924A-6E72E9A43E13}" type="CELLRANGE">
+                    <a:fld id="{0A383941-7261-4A64-AC70-B053987728A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7811,7 +8553,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFD286E3-2D02-4B36-9E6A-6E59260C578F}" type="CELLRANGE">
+                    <a:fld id="{437B03CD-8889-4E30-8823-0D45AC90A11B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7844,7 +8586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31072938-8E44-429D-B86B-B42DC30C485D}" type="CELLRANGE">
+                    <a:fld id="{917C3C37-4497-4E7C-A362-4709BB2C5CEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7877,7 +8619,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9EDEC461-4770-43DC-8CCA-EE53DEAA9BA6}" type="CELLRANGE">
+                    <a:fld id="{2989429E-D19C-4B7D-A479-328C5A220632}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7910,7 +8652,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8511CF7D-C8B3-477D-94F2-4442C0BAB84E}" type="CELLRANGE">
+                    <a:fld id="{5833A2FE-66B7-49F1-AB10-3E2D942244A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9555,7 +10297,7 @@
     <tableColumn id="1" name="P0" dataCellStyle="Currency"/>
     <tableColumn id="2" name="P1" dataCellStyle="Currency"/>
     <tableColumn id="3" name="CashFlows" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="PeriodRet" dataDxfId="352" dataCellStyle="Percent">
+    <tableColumn id="4" name="PeriodRet" dataDxfId="427" dataCellStyle="Percent">
       <calculatedColumnFormula>($B2+$C2)/$A2-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9568,13 +10310,13 @@
   <autoFilter ref="N31:S35"/>
   <tableColumns count="6">
     <tableColumn id="1" name="State" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Probability" totalsRowDxfId="261" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="260" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="259" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="258" totalsRowDxfId="257" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowDxfId="336" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="335" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="334" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="333" totalsRowDxfId="332" dataCellStyle="Percent">
       <calculatedColumnFormula>($P32+$Q32)/160-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="256" totalsRowDxfId="255" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="331" totalsRowDxfId="330" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O32*$R32</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9586,22 +10328,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table378912" displayName="Table378912" ref="O38:V41" totalsRowCount="1">
   <autoFilter ref="O38:V40"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="254" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="253" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="252" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="251" totalsRowDxfId="250" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="329" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="328" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="327" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="326" totalsRowDxfId="325" dataCellStyle="Percent">
       <calculatedColumnFormula>($P39+$Q39)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="249" totalsRowDxfId="248" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="324" totalsRowDxfId="323" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O39*$R39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="247" totalsRowDxfId="246" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="322" totalsRowDxfId="321" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R39-$S$41,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="245" totalsRowDxfId="244" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="320" totalsRowDxfId="319" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T39*$O39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="243" totalsRowDxfId="242" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="318" totalsRowDxfId="317" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U41)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -9614,53 +10356,53 @@
   <autoFilter ref="A1:T5"/>
   <tableColumns count="20">
     <tableColumn id="1" name="State" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="241" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Toyota" dataDxfId="240" totalsRowDxfId="239" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Walmart" dataDxfId="238" totalsRowDxfId="237" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Pfizer" dataDxfId="236" totalsRowDxfId="235" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Twted" totalsRowFunction="sum" dataDxfId="234" totalsRowDxfId="233" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="316" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Toyota" dataDxfId="315" totalsRowDxfId="314" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Walmart" dataDxfId="313" totalsRowDxfId="312" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Pfizer" dataDxfId="311" totalsRowDxfId="310" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Twted" totalsRowFunction="sum" dataDxfId="309" totalsRowDxfId="308" dataCellStyle="Percent">
       <calculatedColumnFormula>C2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WMTwted" totalsRowFunction="sum" dataDxfId="232" totalsRowDxfId="231" dataCellStyle="Percent">
+    <tableColumn id="7" name="WMTwted" totalsRowFunction="sum" dataDxfId="307" totalsRowDxfId="306" dataCellStyle="Percent">
       <calculatedColumnFormula>D2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PFZwted" totalsRowFunction="sum" dataDxfId="230" totalsRowDxfId="229" dataCellStyle="Percent">
+    <tableColumn id="8" name="PFZwted" totalsRowFunction="sum" dataDxfId="305" totalsRowDxfId="304" dataCellStyle="Percent">
       <calculatedColumnFormula>E2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Tvar" totalsRowFunction="sum" dataDxfId="228" totalsRowDxfId="227" dataCellStyle="Percent">
+    <tableColumn id="16" name="Tvar" totalsRowFunction="sum" dataDxfId="303" totalsRowDxfId="302" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(C2-F$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Wvar" totalsRowFunction="sum" dataDxfId="226" totalsRowDxfId="225" dataCellStyle="Percent">
+    <tableColumn id="15" name="Wvar" totalsRowFunction="sum" dataDxfId="301" totalsRowDxfId="300" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(D2-G$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Pvar" totalsRowFunction="sum" dataDxfId="224" totalsRowDxfId="223" dataCellStyle="Percent">
+    <tableColumn id="14" name="Pvar" totalsRowFunction="sum" dataDxfId="299" totalsRowDxfId="298" dataCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(E2-H$6,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixT" dataDxfId="222" totalsRowDxfId="221" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixT" dataDxfId="297" totalsRowDxfId="296" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixWMT" dataDxfId="220" totalsRowDxfId="219" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixWMT" dataDxfId="295" totalsRowDxfId="294" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixPFZ" dataDxfId="218" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixPFZ" dataDxfId="293" dataCellStyle="Percent">
       <calculatedColumnFormula>1-L2-M2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="217" totalsRowDxfId="216" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="292" totalsRowDxfId="291" dataCellStyle="Percent">
       <calculatedColumnFormula>C2*L$2+D2*M$2+E2*N$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="215" totalsRowDxfId="214" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="290" totalsRowDxfId="289" dataCellStyle="Percent">
       <calculatedColumnFormula>O2*$B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="MixVar" totalsRowFunction="sum" dataDxfId="213" totalsRowDxfId="212" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="17" name="MixVar" totalsRowFunction="sum" dataDxfId="288" totalsRowDxfId="287" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$B2*POWER(O2-$P$6, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Wpcov" totalsRowFunction="sum" dataDxfId="211" totalsRowDxfId="210" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="18" name="Wpcov" totalsRowFunction="sum" dataDxfId="286" totalsRowDxfId="285" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(D2-G$6)*(E2-H$6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Tpcov" totalsRowFunction="sum" dataDxfId="209" totalsRowDxfId="208" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="19" name="Tpcov" totalsRowFunction="sum" dataDxfId="284" totalsRowDxfId="283" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(C2-F$6)*(E2-H$6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="Twcov" totalsRowFunction="sum" dataDxfId="207" totalsRowDxfId="206" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="20" name="Twcov" totalsRowFunction="sum" dataDxfId="282" totalsRowDxfId="281" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$B2*(C2-F$6)*(D2-G$6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9672,53 +10414,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1214" displayName="Table1214" ref="V1:AN5" totalsRowCount="1">
   <autoFilter ref="V1:AN4"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="205" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="204" totalsRowDxfId="203" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="202" totalsRowDxfId="201" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="200" totalsRowDxfId="199" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="198" totalsRowDxfId="197" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="280" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="273" totalsRowDxfId="272" dataCellStyle="Percent">
       <calculatedColumnFormula>W2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="196" totalsRowDxfId="195" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="271" totalsRowDxfId="270" dataCellStyle="Percent">
       <calculatedColumnFormula>X2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="194" totalsRowDxfId="193" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="269" totalsRowDxfId="268" dataCellStyle="Percent">
       <calculatedColumnFormula>Y2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="192" totalsRowDxfId="191" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="267" totalsRowDxfId="266" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(W2-Z$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="190" totalsRowDxfId="189" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="265" totalsRowDxfId="264" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(X2-AA$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="188" totalsRowDxfId="187" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="263" totalsRowDxfId="262" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(Y2-AB$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="186" totalsRowDxfId="185" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="261" totalsRowDxfId="260" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="184" totalsRowDxfId="183" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="259" totalsRowDxfId="258" dataCellStyle="Percent">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="182" totalsRowDxfId="181" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="257" totalsRowDxfId="256" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF2-AG2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="180" totalsRowDxfId="179" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="255" totalsRowDxfId="254" dataCellStyle="Percent">
       <calculatedColumnFormula>W2*AF$2+X2*AG$2+Y2*AH$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="178" totalsRowDxfId="177" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="253" totalsRowDxfId="252" dataCellStyle="Percent">
       <calculatedColumnFormula>AI2*$V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="176" totalsRowDxfId="175" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="251" totalsRowDxfId="250" dataCellStyle="Percent">
       <calculatedColumnFormula>$V2*POWER(AI2-AJ$5,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="174" totalsRowDxfId="173" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="249" totalsRowDxfId="248" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(W2-Z$5)*(X2-AA$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="172" totalsRowDxfId="171" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="247" totalsRowDxfId="246" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(W2-Z$5)*(Y2-AB$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="170" totalsRowDxfId="169" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="245" totalsRowDxfId="244" dataCellStyle="Comma">
       <calculatedColumnFormula>$V2*(X2-AA$5)*(Y2-AB$5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9731,9 +10473,9 @@
   <autoFilter ref="AP1:AS4"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Label" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="ExpRet" dataDxfId="168" totalsRowDxfId="167" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
-    <tableColumn id="3" name="Wt" totalsRowDxfId="166" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
-    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="165" totalsRowDxfId="164" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="2" name="ExpRet" dataDxfId="243" totalsRowDxfId="242" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
+    <tableColumn id="3" name="Wt" totalsRowDxfId="241" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
+    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="240" totalsRowDxfId="239" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>AQ2*AR2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9746,9 +10488,9 @@
   <autoFilter ref="AP8:AS11"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Label" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="ExpRet" dataDxfId="163" totalsRowDxfId="162" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
-    <tableColumn id="3" name="Wt" totalsRowDxfId="161" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
-    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="160" totalsRowDxfId="159" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="2" name="ExpRet" dataDxfId="238" totalsRowDxfId="237" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
+    <tableColumn id="3" name="Wt" totalsRowDxfId="236" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
+    <tableColumn id="4" name="WtdRet" totalsRowFunction="sum" dataDxfId="235" totalsRowDxfId="234" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>AQ9*AR9</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9762,8 +10504,8 @@
   <tableColumns count="9">
     <tableColumn id="1" name="Capital" dataCellStyle="Currency"/>
     <tableColumn id="2" name="Borrowed" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="LoanInt" dataDxfId="158" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Ret" dataDxfId="157" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="LoanInt" dataDxfId="233" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Ret" dataDxfId="232" dataCellStyle="Percent"/>
     <tableColumn id="5" name="TotInv">
       <calculatedColumnFormula>AU2+AV2</calculatedColumnFormula>
     </tableColumn>
@@ -9776,7 +10518,7 @@
     <tableColumn id="8" name="NetRetVal">
       <calculatedColumnFormula>AZ2-BA2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="RetRate" dataDxfId="156" dataCellStyle="Percent">
+    <tableColumn id="9" name="RetRate" dataDxfId="231" dataCellStyle="Percent">
       <calculatedColumnFormula>BB2/AU2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9788,53 +10530,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table121417" displayName="Table121417" ref="V9:AN13" totalsRowCount="1">
   <autoFilter ref="V9:AN12"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="155" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="154" totalsRowDxfId="153" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="152" totalsRowDxfId="151" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="148" totalsRowDxfId="147" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="230" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="229" totalsRowDxfId="228" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="227" totalsRowDxfId="226" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="225" totalsRowDxfId="224" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="223" totalsRowDxfId="222" dataCellStyle="Percent">
       <calculatedColumnFormula>W10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="146" totalsRowDxfId="145" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="221" totalsRowDxfId="220" dataCellStyle="Percent">
       <calculatedColumnFormula>X10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="144" totalsRowDxfId="143" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="219" totalsRowDxfId="218" dataCellStyle="Percent">
       <calculatedColumnFormula>Y10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="142" totalsRowDxfId="141" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="217" totalsRowDxfId="216" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(W10-Z$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="140" totalsRowDxfId="139" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="215" totalsRowDxfId="214" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(X10-AA$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="138" totalsRowDxfId="137" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="213" totalsRowDxfId="212" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(Y10-AB$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="136" totalsRowDxfId="135" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="211" totalsRowDxfId="210" dataCellStyle="Percent">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="134" totalsRowDxfId="133" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="209" totalsRowDxfId="208" dataCellStyle="Percent">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="132" totalsRowDxfId="131" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="207" totalsRowDxfId="206" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF10-AG10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="130" totalsRowDxfId="129" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="205" totalsRowDxfId="204" dataCellStyle="Percent">
       <calculatedColumnFormula>W10*AF$2+X10*AG$2+Y10*AH$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="203" totalsRowDxfId="202" dataCellStyle="Percent">
       <calculatedColumnFormula>AI10*$V10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="201" totalsRowDxfId="200" dataCellStyle="Percent">
       <calculatedColumnFormula>$V10*POWER(AI10-AJ$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="124" totalsRowDxfId="123" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="199" totalsRowDxfId="198" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(W10-Z$13)*(X10-AA$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="122" totalsRowDxfId="121" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="197" totalsRowDxfId="196" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(W10-Z$13)*(Y10-AB$13)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="120" totalsRowDxfId="119" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="195" totalsRowDxfId="194" dataCellStyle="Comma">
       <calculatedColumnFormula>$V10*(X10-AA$13)*(Y10-AB$13)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9846,22 +10588,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="BE1:BQ2" totalsRowShown="0">
   <autoFilter ref="BE1:BQ2"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Jret" dataDxfId="118" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="Rret" dataDxfId="117" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Jret" dataDxfId="193" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="Rret" dataDxfId="192" dataCellStyle="Percent"/>
     <tableColumn id="3" name="Jwt"/>
     <tableColumn id="4" name="Rwt">
       <calculatedColumnFormula>1-BG2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="ExpRet" dataDxfId="116" dataCellStyle="Percent">
+    <tableColumn id="5" name="ExpRet" dataDxfId="191" dataCellStyle="Percent">
       <calculatedColumnFormula>BE2*BG2+BF2*BH2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Jvol" dataDxfId="115" dataCellStyle="Percent"/>
-    <tableColumn id="7" name="Rvol" dataDxfId="114" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Jrcorr" dataDxfId="113" dataCellStyle="Comma"/>
-    <tableColumn id="9" name="Jvar" dataDxfId="112" dataCellStyle="Percent">
+    <tableColumn id="6" name="Jvol" dataDxfId="190" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Rvol" dataDxfId="189" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Jrcorr" dataDxfId="188" dataCellStyle="Comma"/>
+    <tableColumn id="9" name="Jvar" dataDxfId="187" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BJ2,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Rvar" dataDxfId="111" dataCellStyle="Percent">
+    <tableColumn id="10" name="Rvar" dataDxfId="186" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BK2,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Jrcov">
@@ -9870,7 +10612,7 @@
     <tableColumn id="12" name="Jrvar">
       <calculatedColumnFormula>BM2*BG2*BG2+BN2*BH2*BH2+2*BG2*BH2*BO2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Jrvol" dataDxfId="110" dataCellStyle="Percent">
+    <tableColumn id="13" name="Jrvol" dataDxfId="185" dataCellStyle="Percent">
       <calculatedColumnFormula>SQRT(BP2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9882,24 +10624,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1820" displayName="Table1820" ref="BE6:BQ7" totalsRowShown="0">
   <autoFilter ref="BE6:BQ7"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Jret" dataDxfId="109" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="Rret" dataDxfId="108" dataCellStyle="Percent"/>
+    <tableColumn id="1" name="Jret" dataDxfId="184" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="Rret" dataDxfId="183" dataCellStyle="Percent"/>
     <tableColumn id="3" name="Jwt">
       <calculatedColumnFormula>1/2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Rwt">
       <calculatedColumnFormula>1-BG7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="ExpRet" dataDxfId="107" dataCellStyle="Percent">
+    <tableColumn id="5" name="ExpRet" dataDxfId="182" dataCellStyle="Percent">
       <calculatedColumnFormula>BE7*BG7+BF7*BH7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Jvol" dataDxfId="106" dataCellStyle="Percent"/>
-    <tableColumn id="7" name="Rvol" dataDxfId="105" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Jrcorr" dataDxfId="104" dataCellStyle="Comma"/>
-    <tableColumn id="9" name="Jvar" dataDxfId="103" dataCellStyle="Percent">
+    <tableColumn id="6" name="Jvol" dataDxfId="181" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Rvol" dataDxfId="180" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Jrcorr" dataDxfId="179" dataCellStyle="Comma"/>
+    <tableColumn id="9" name="Jvar" dataDxfId="178" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BJ7,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Rvar" dataDxfId="102" dataCellStyle="Percent">
+    <tableColumn id="10" name="Rvar" dataDxfId="177" dataCellStyle="Percent">
       <calculatedColumnFormula>POWER(BK7,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" name="Jrcov">
@@ -9908,7 +10650,7 @@
     <tableColumn id="12" name="Jrvar">
       <calculatedColumnFormula>BM7*BG7*BG7+BN7*BH7*BH7+2*BG7*BH7*BO7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Jrvol" dataDxfId="101" dataCellStyle="Percent">
+    <tableColumn id="13" name="Jrvol" dataDxfId="176" dataCellStyle="Percent">
       <calculatedColumnFormula>SQRT(BP7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9921,20 +10663,20 @@
   <autoFilter ref="F1:L6"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="351" totalsRowDxfId="350" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="349" totalsRowDxfId="348" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="426" totalsRowDxfId="425" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="424" totalsRowDxfId="423" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="347" totalsRowDxfId="346" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="422" totalsRowDxfId="421" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$2:$H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="345" totalsRowDxfId="344" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="420" totalsRowDxfId="419" dataCellStyle="Percent">
       <calculatedColumnFormula>$I2-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="343" totalsRowDxfId="342" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="418" totalsRowDxfId="417" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$2:$H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="341" totalsRowDxfId="340" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="416" totalsRowDxfId="415" dataCellStyle="Percent">
       <calculatedColumnFormula>$K2-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9947,12 +10689,12 @@
   <autoFilter ref="BS1:BW4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Security" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Ret" dataDxfId="100" totalsRowDxfId="99" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="Invested" totalsRowFunction="sum" totalsRowDxfId="98" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Wt" dataDxfId="97" totalsRowDxfId="96" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="175" totalsRowDxfId="174" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="Invested" totalsRowFunction="sum" totalsRowDxfId="173" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Wt" dataDxfId="172" totalsRowDxfId="171" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>BU2/BU$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="WtdRet" totalsRowFunction="sum" dataDxfId="95" totalsRowDxfId="94" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="WtdRet" totalsRowFunction="sum" dataDxfId="170" totalsRowDxfId="169" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>BT2*BV2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9964,53 +10706,53 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table12141723" displayName="Table12141723" ref="V17:AN21" totalsRowCount="1">
   <autoFilter ref="V17:AN20"/>
   <tableColumns count="19">
-    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="93" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="ARet " dataDxfId="92" totalsRowDxfId="91" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Bret" dataDxfId="90" totalsRowDxfId="89" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Cret" dataDxfId="88" totalsRowDxfId="87" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Percent">
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum" totalsRowDxfId="168" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="ARet " dataDxfId="167" totalsRowDxfId="166" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Bret" dataDxfId="165" totalsRowDxfId="164" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Cret" dataDxfId="163" totalsRowDxfId="162" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="Awted" totalsRowFunction="sum" dataDxfId="161" totalsRowDxfId="160" dataCellStyle="Percent">
       <calculatedColumnFormula>W18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Percent">
+    <tableColumn id="7" name="Bwted" totalsRowFunction="sum" dataDxfId="159" totalsRowDxfId="158" dataCellStyle="Percent">
       <calculatedColumnFormula>X18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="82" totalsRowDxfId="81" dataCellStyle="Percent">
+    <tableColumn id="8" name="Cwted" totalsRowFunction="sum" dataDxfId="157" totalsRowDxfId="156" dataCellStyle="Percent">
       <calculatedColumnFormula>Y18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="80" totalsRowDxfId="79" dataCellStyle="Percent">
+    <tableColumn id="15" name="Avar" totalsRowFunction="sum" dataDxfId="155" totalsRowDxfId="154" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(W18-Z$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="78" totalsRowDxfId="77" dataCellStyle="Percent">
+    <tableColumn id="14" name="Bvar" totalsRowFunction="sum" dataDxfId="153" totalsRowDxfId="152" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(X18-AA$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="75" dataCellStyle="Percent">
+    <tableColumn id="1" name="Cvar" totalsRowFunction="sum" dataDxfId="151" totalsRowDxfId="150" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(Y18-AB$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="MixA" dataDxfId="74" totalsRowDxfId="73" dataCellStyle="Percent">
+    <tableColumn id="9" name="MixA" dataDxfId="149" totalsRowDxfId="148" dataCellStyle="Percent">
       <calculatedColumnFormula>0.6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="MixB" dataDxfId="72" totalsRowDxfId="71" dataCellStyle="Percent">
+    <tableColumn id="10" name="MixB" dataDxfId="147" totalsRowDxfId="146" dataCellStyle="Percent">
       <calculatedColumnFormula>0.4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="MixC" dataDxfId="70" totalsRowDxfId="69" dataCellStyle="Percent">
+    <tableColumn id="11" name="MixC" dataDxfId="145" totalsRowDxfId="144" dataCellStyle="Percent">
       <calculatedColumnFormula>1-AF18-AG18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="MixRet" dataDxfId="68" totalsRowDxfId="67" dataCellStyle="Percent">
+    <tableColumn id="12" name="MixRet" dataDxfId="143" totalsRowDxfId="142" dataCellStyle="Percent">
       <calculatedColumnFormula>W18*AF$18+X18*AG$18+Y18*AH$18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="66" totalsRowDxfId="65" dataCellStyle="Percent">
+    <tableColumn id="13" name="MixWted" totalsRowFunction="sum" dataDxfId="141" totalsRowDxfId="140" dataCellStyle="Percent">
       <calculatedColumnFormula>AI18*$V18</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="64" totalsRowDxfId="63" dataCellStyle="Percent">
+    <tableColumn id="16" name="MixVar" totalsRowFunction="sum" dataDxfId="139" totalsRowDxfId="138" dataCellStyle="Percent">
       <calculatedColumnFormula>$V18*POWER(AI18-AJ$21,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61" dataCellStyle="Comma">
+    <tableColumn id="17" name="Abcov" totalsRowFunction="sum" dataDxfId="137" totalsRowDxfId="136" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(W18-Z$21)*(X18-AA$21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59" dataCellStyle="Comma">
+    <tableColumn id="18" name="Accov" totalsRowFunction="sum" dataDxfId="135" totalsRowDxfId="134" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(W18-Z$21)*(Y18-AB$21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57" dataCellStyle="Comma">
+    <tableColumn id="19" name="Bccov" totalsRowFunction="sum" dataDxfId="133" totalsRowDxfId="132" dataCellStyle="Comma">
       <calculatedColumnFormula>$V18*(X18-AA$21)*(Y18-AB$21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10035,7 +10777,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="A2:B3" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2" dataDxfId="56" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Column2" dataDxfId="131" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10046,12 +10788,12 @@
   <autoFilter ref="A4:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Investment"/>
-    <tableColumn id="2" name="Ret" dataDxfId="55" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="SD" dataDxfId="54" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Var" dataDxfId="53" dataCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="130" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="129" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="128" dataCellStyle="Comma">
       <calculatedColumnFormula>C5*C5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Utility" dataDxfId="52" dataCellStyle="Comma">
+    <tableColumn id="5" name="Utility" dataDxfId="127" dataCellStyle="Comma">
       <calculatedColumnFormula>B5-0.5*$B$2*D5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10064,12 +10806,12 @@
   <autoFilter ref="A9:E11"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Investment"/>
-    <tableColumn id="2" name="Ret" dataDxfId="51" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="SD" dataDxfId="50" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Var" dataDxfId="49" dataCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="126" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="125" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="124" dataCellStyle="Comma">
       <calculatedColumnFormula>C10*C10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Utility" dataDxfId="48" dataCellStyle="Comma">
+    <tableColumn id="5" name="Utility" dataDxfId="123" dataCellStyle="Comma">
       <calculatedColumnFormula>B10-0.5*$B$2*D10</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10084,17 +10826,17 @@
     <tableColumn id="1" name="Investment"/>
     <tableColumn id="2" name="W1" dataCellStyle="Currency"/>
     <tableColumn id="3" name="W2" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="P1" dataDxfId="47" dataCellStyle="Comma"/>
-    <tableColumn id="5" name="P2" dataDxfId="46" dataCellStyle="Comma">
+    <tableColumn id="4" name="P1" dataDxfId="122" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="P2" dataDxfId="121" dataCellStyle="Comma">
       <calculatedColumnFormula>1-J5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="U1" dataDxfId="45">
+    <tableColumn id="6" name="U1" dataDxfId="120">
       <calculatedColumnFormula>LN(H5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="U2">
       <calculatedColumnFormula>LN(I5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="EU" dataDxfId="44">
+    <tableColumn id="8" name="EU" dataDxfId="119">
       <calculatedColumnFormula>J5*L5+K5*M5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10107,12 +10849,12 @@
   <autoFilter ref="A13:E16"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Investment"/>
-    <tableColumn id="2" name="Ret" dataDxfId="43" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="SD" dataDxfId="42" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Var" dataDxfId="41" dataCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="118" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="117" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="116" dataCellStyle="Comma">
       <calculatedColumnFormula>C14*C14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Utility" dataDxfId="40" dataCellStyle="Comma">
+    <tableColumn id="5" name="Utility" dataDxfId="115" dataCellStyle="Comma">
       <calculatedColumnFormula>B14-0.5*$B$2*D14</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10124,10 +10866,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="A1:D3" totalsRowShown="0">
   <autoFilter ref="A1:D3"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ExpRet" dataDxfId="39" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="SD" dataDxfId="38" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="RiskFreeRate" dataDxfId="37" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="SharpeRatio" dataDxfId="36">
+    <tableColumn id="1" name="ExpRet" dataDxfId="114" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="SD" dataDxfId="113" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="RiskFreeRate" dataDxfId="112" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="SharpeRatio" dataDxfId="111">
       <calculatedColumnFormula>(A2-C2)/B2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10136,17 +10878,17 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table29" displayName="Table29" ref="F1:K4" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" headerRowCellStyle="Percent" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table29" displayName="Table29" ref="F1:K4" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" headerRowCellStyle="Percent" dataCellStyle="Percent">
   <autoFilter ref="F1:K4"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ExpExcessRet" dataDxfId="33" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="SD" dataDxfId="32" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="RiskFreeRate" dataDxfId="31" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="A" dataDxfId="30" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Var" dataDxfId="29" dataCellStyle="Percent">
+    <tableColumn id="1" name="ExpExcessRet" dataDxfId="108" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="SD" dataDxfId="107" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="RiskFreeRate" dataDxfId="106" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="A" dataDxfId="105" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Var" dataDxfId="104" dataCellStyle="Percent">
       <calculatedColumnFormula>G2*G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="w" dataDxfId="28" dataCellStyle="Percent">
+    <tableColumn id="6" name="w" dataDxfId="103" dataCellStyle="Percent">
       <calculatedColumnFormula>F2/(I2*J2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10162,10 +10904,10 @@
     <tableColumn id="2" name="Probability" dataCellStyle="Comma" totalsRowCellStyle="Comma"/>
     <tableColumn id="3" name="YrEndPrice" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
     <tableColumn id="4" name="CashFlow" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="339" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="5" name="Ret" dataDxfId="414" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>($P2+$Q2)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="338" totalsRowDxfId="337" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="413" totalsRowDxfId="412" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O2*$R2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10177,10 +10919,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table30" displayName="Table30" ref="M1:P2" totalsRowShown="0">
   <autoFilter ref="M1:P2"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="RiskyRet" dataDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="RiskFreeRet" dataDxfId="26" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="TargetRet" dataDxfId="25" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="wRisky" dataDxfId="24" dataCellStyle="Comma">
+    <tableColumn id="1" name="RiskyRet" dataDxfId="102" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="RiskFreeRet" dataDxfId="101" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="TargetRet" dataDxfId="100" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="wRisky" dataDxfId="99" dataCellStyle="Comma">
       <calculatedColumnFormula>(O2-N2)/(M2-N2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10192,9 +10934,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table31" displayName="Table31" ref="R1:T3" totalsRowShown="0">
   <autoFilter ref="R1:T3"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="RiskySD" dataDxfId="23" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="TargetSD" dataDxfId="22" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="wRisky" dataDxfId="21" dataCellStyle="Percent">
+    <tableColumn id="1" name="RiskySD" dataDxfId="98" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="TargetSD" dataDxfId="97" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="wRisky" dataDxfId="96" dataCellStyle="Percent">
       <calculatedColumnFormula>S2/R2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10206,14 +10948,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Table32" displayName="Table32" ref="V1:AA2" totalsRowShown="0">
   <autoFilter ref="V1:AA2"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="riskySD" dataDxfId="20" dataCellStyle="Percent"/>
-    <tableColumn id="2" name="riskyRet" dataDxfId="19" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="riskFreeRet" dataDxfId="18" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="targSD" dataDxfId="17" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="riskyWt" dataDxfId="16" dataCellStyle="Comma">
+    <tableColumn id="1" name="riskySD" dataDxfId="95" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="riskyRet" dataDxfId="94" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="riskFreeRet" dataDxfId="93" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="targSD" dataDxfId="92" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="riskyWt" dataDxfId="91" dataCellStyle="Comma">
       <calculatedColumnFormula>Y2/V2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="pfRet" dataDxfId="15" dataCellStyle="Percent">
+    <tableColumn id="6" name="pfRet" dataDxfId="90" dataCellStyle="Percent">
       <calculatedColumnFormula>Z2*W2+(1-Z2)*X2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10225,18 +10967,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Table33" displayName="Table33" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="DivInv" dataDxfId="14" dataCellStyle="Currency"/>
-    <tableColumn id="2" name="FelixInv" dataDxfId="13" dataCellStyle="Currency"/>
-    <tableColumn id="3" name="Total" dataDxfId="12" dataCellStyle="Currency">
+    <tableColumn id="1" name="DivInv" dataDxfId="89" dataCellStyle="Currency"/>
+    <tableColumn id="2" name="FelixInv" dataDxfId="88" dataCellStyle="Currency"/>
+    <tableColumn id="3" name="Total" dataDxfId="87" dataCellStyle="Currency">
       <calculatedColumnFormula>A2+B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="DivWt" dataDxfId="11" dataCellStyle="Comma">
+    <tableColumn id="4" name="DivWt" dataDxfId="86" dataCellStyle="Comma">
       <calculatedColumnFormula>A2/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="FelixWt" dataDxfId="10" dataCellStyle="Comma">
+    <tableColumn id="5" name="FelixWt" dataDxfId="85" dataCellStyle="Comma">
       <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="TotWt" dataDxfId="9" dataCellStyle="Comma">
+    <tableColumn id="6" name="TotWt" dataDxfId="84" dataCellStyle="Comma">
       <calculatedColumnFormula>D2+E2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10249,9 +10991,9 @@
   <autoFilter ref="H1:K3"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Desc"/>
-    <tableColumn id="2" name="Ret" dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="SD" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Var" dataDxfId="3" dataCellStyle="Comma">
+    <tableColumn id="2" name="Ret" dataDxfId="83" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="SD" dataDxfId="82" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Var" dataDxfId="81" dataCellStyle="Comma">
       <calculatedColumnFormula>J2*J2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10260,10 +11002,10 @@
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="Table35" displayName="Table35" ref="M1:M2" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowCellStyle="Percent" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="Table35" displayName="Table35" ref="M1:M2" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" headerRowCellStyle="Percent" dataCellStyle="Percent">
   <autoFilter ref="M1:M2"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="pfRet" dataDxfId="7" dataCellStyle="Percent">
+    <tableColumn id="1" name="pfRet" dataDxfId="78" dataCellStyle="Percent">
       <calculatedColumnFormula>D2*I2+E2*I3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10272,15 +11014,88 @@
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="Table36" displayName="Table36" ref="O1:P2" totalsRowShown="0" dataDxfId="0" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="Table36" displayName="Table36" ref="O1:P2" totalsRowShown="0" dataDxfId="77" dataCellStyle="Comma">
   <autoFilter ref="O1:P2"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Corr" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Cov" dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="1" name="Corr" dataDxfId="76" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Cov" dataDxfId="75" dataCellStyle="Comma">
       <calculatedColumnFormula>O2*J2*J3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Table38" displayName="Table38" ref="A1:G2" totalsRowShown="0">
+  <autoFilter ref="A1:G2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="RisklessRate" dataDxfId="74" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="RiskyRate" dataDxfId="73" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="RiskyVol" dataDxfId="72" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="RiskyPortion" dataDxfId="71" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="ExcessRate">
+      <calculatedColumnFormula>B2-A2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="RiskyVar" dataDxfId="70" dataCellStyle="Comma">
+      <calculatedColumnFormula>C2*C2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="AveGamma" dataDxfId="69" dataCellStyle="Comma">
+      <calculatedColumnFormula>E2/(D2*F2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="Table39" displayName="Table39" ref="I1:R2" totalsRowShown="0">
+  <autoFilter ref="I1:R2"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="RisklessRate" dataDxfId="68" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="MktPfRet" dataDxfId="67" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="MktPfVar" dataDxfId="66" dataCellStyle="Comma"/>
+    <tableColumn id="4" name="VarZ" dataDxfId="65" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="CorrMktZ" dataDxfId="64" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="VolMkt" dataDxfId="63" dataCellStyle="Percent">
+      <calculatedColumnFormula>SQRT(K2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="VolZ" dataDxfId="62" dataCellStyle="Percent">
+      <calculatedColumnFormula>SQRT(L2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="MktExcessRet" dataDxfId="61" dataCellStyle="Percent">
+      <calculatedColumnFormula>J2-I2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="BetaZ" dataDxfId="60" dataCellStyle="Comma">
+      <calculatedColumnFormula>M2*O2/N2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="Zret" dataDxfId="59" dataCellStyle="Percent">
+      <calculatedColumnFormula>I2+Q2*P2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="Table3940" displayName="Table3940" ref="T1:Z2" totalsRowShown="0">
+  <autoFilter ref="T1:Z2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="RisklessRate" dataDxfId="58" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="MktPfRet" dataDxfId="57" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="MktPfVol" dataDxfId="56" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="TargRet" dataDxfId="55" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="MktExcessRet" dataDxfId="54" dataCellStyle="Percent">
+      <calculatedColumnFormula>U2-T2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="TargExcessRet" dataDxfId="53" dataCellStyle="Percent">
+      <calculatedColumnFormula>W2-T2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="TargVol" dataDxfId="52" dataCellStyle="Percent">
+      <calculatedColumnFormula>V2*Y2/X2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -10289,20 +11104,20 @@
   <autoFilter ref="F9:L12"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="336" totalsRowDxfId="335" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="334" totalsRowDxfId="333" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="411" totalsRowDxfId="410" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="409" totalsRowDxfId="408" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="332" totalsRowDxfId="331" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="407" totalsRowDxfId="406" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$10:$H10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="330" totalsRowDxfId="329" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="405" totalsRowDxfId="404" dataCellStyle="Percent">
       <calculatedColumnFormula>$I10-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="328" totalsRowDxfId="327" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="403" totalsRowDxfId="402" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$10:$H10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="326" totalsRowDxfId="325" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="401" totalsRowDxfId="400" dataCellStyle="Percent">
       <calculatedColumnFormula>$K10-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10310,26 +11125,209 @@
 </table>
 </file>
 
+<file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="40" name="Table394041" displayName="Table394041" ref="AB1:AH2" totalsRowShown="0">
+  <autoFilter ref="AB1:AH2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="RisklessRate" dataDxfId="51" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="MktPfRet" dataDxfId="50" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="MktPfVol" dataDxfId="49" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="TargVol" dataDxfId="48" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="MktExcessRet" dataDxfId="47" dataCellStyle="Percent">
+      <calculatedColumnFormula>AC2-AB2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="TargExcessRet" dataDxfId="46" dataCellStyle="Percent">
+      <calculatedColumnFormula>AF2*AE2/AD2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="TargRet" dataDxfId="45" dataCellStyle="Percent">
+      <calculatedColumnFormula>AG2+AB2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="AN1:AT6" totalsRowCount="1">
+  <autoFilter ref="AN1:AT5"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Security" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Invested" totalsRowFunction="sum" totalsRowDxfId="44" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
+    <tableColumn id="3" name="Beta"/>
+    <tableColumn id="4" name="Weight" totalsRowFunction="sum" dataDxfId="43">
+      <calculatedColumnFormula>AO2/AO$6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="BetaWtdAve" totalsRowFunction="sum" dataDxfId="42">
+      <calculatedColumnFormula>AP2*AQ2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Ret" dataDxfId="41" totalsRowDxfId="40" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>$AJ$2+AP2*$AL$2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="RetWtdAve" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>AQ2*AS2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="AJ1:AL2" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" headerRowCellStyle="Percent" dataCellStyle="Percent">
+  <autoFilter ref="AJ1:AL2"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="RisklessRate" dataDxfId="35" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="MktRate" dataDxfId="34" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="MktExcessRate" dataDxfId="33" dataCellStyle="Percent">
+      <calculatedColumnFormula>AK2-AJ2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="43" name="Table43" displayName="Table43" ref="AV1:BA5" totalsRowCount="1">
+  <autoFilter ref="AV1:BA4"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Condition" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum"/>
+    <tableColumn id="3" name="Aprice" totalsRowDxfId="32" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Ret" dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>AX2/50-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="RetWtdAve" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>AW2*AY2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="VarSub" totalsRowFunction="sum" dataDxfId="27">
+      <calculatedColumnFormula>AW2*POWER(AY2-AZ$5,2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="44" name="Table44" displayName="Table44" ref="BC1:BF4" totalsRowShown="0">
+  <autoFilter ref="BC1:BF4"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="MktVol" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="2" name="StockVol" dataDxfId="25">
+      <calculatedColumnFormula>BA6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Corr"/>
+    <tableColumn id="4" name="StockBeta" dataDxfId="24" dataCellStyle="Comma">
+      <calculatedColumnFormula>BE2*BD2/BC2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table45.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="45" name="Table45" displayName="Table45" ref="BH1:BM2" totalsRowShown="0">
+  <autoFilter ref="BH1:BM2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="StockBeta"/>
+    <tableColumn id="2" name="RisklessRet" dataDxfId="23" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="MktRet" dataDxfId="22" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="MktExcessRet">
+      <calculatedColumnFormula>BJ2-BI2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="StockExcessRet" dataDxfId="21" dataCellStyle="Percent">
+      <calculatedColumnFormula>BH2*BK2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="StockRet" dataDxfId="20" dataCellStyle="Percent">
+      <calculatedColumnFormula>BL2+BI2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table46.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="47" name="Table4348" displayName="Table4348" ref="AV8:BA12" totalsRowCount="1">
+  <autoFilter ref="AV8:BA11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Condition" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum"/>
+    <tableColumn id="3" name="Aprice" totalsRowDxfId="19" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Ret" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>AX9/50-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="RetWtdAve" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>AW9*AY9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="VarSub" totalsRowFunction="sum" dataDxfId="14">
+      <calculatedColumnFormula>AW9*POWER(AY9-AZ$12,2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table47.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="48" name="Table434849" displayName="Table434849" ref="AV15:BA19" totalsRowCount="1">
+  <autoFilter ref="AV15:BA18"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Condition" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Prob" totalsRowFunction="sum"/>
+    <tableColumn id="3" name="Bprice" totalsRowDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Ret" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>AX16/50-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="RetWtdAve" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>AW16*AY16</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="VarSub" totalsRowFunction="sum" dataDxfId="8">
+      <calculatedColumnFormula>AW16*POWER(AY16-AZ$12,2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table48.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="46" name="Table46" displayName="Table46" ref="A1:I2" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowCellStyle="Percent" dataCellStyle="Percent">
+  <autoFilter ref="A1:I2"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Bmkt"/>
+    <tableColumn id="2" name="Bsmb"/>
+    <tableColumn id="3" name="Bhml"/>
+    <tableColumn id="4" name="Mkt-rf" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="SMB" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="HML" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="rf" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="MonthlyRet" dataDxfId="1">
+      <calculatedColumnFormula>G2+SUMPRODUCT(A2:C2,D2:F2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="YrlyRet" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>12*H2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="O9:V13" totalsRowCount="1">
   <autoFilter ref="O9:V12"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="324" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="323" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="322" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="321" totalsRowDxfId="320" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="399" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="398" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="397" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="396" totalsRowDxfId="395" dataCellStyle="Percent">
       <calculatedColumnFormula>($P10+$Q10)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="319" totalsRowDxfId="318" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="394" totalsRowDxfId="393" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O10*$R10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="317" totalsRowDxfId="316" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="392" totalsRowDxfId="391" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R10-$S$13,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="315" totalsRowDxfId="314" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="390" totalsRowDxfId="389" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T10*$O10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="313" totalsRowDxfId="312" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="388" totalsRowDxfId="387" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U13)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -10341,22 +11339,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table378" displayName="Table378" ref="O16:V20" totalsRowCount="1">
   <autoFilter ref="O16:V19"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="311" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="310" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="309" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="308" totalsRowDxfId="307" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="386" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="385" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="384" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="383" totalsRowDxfId="382" dataCellStyle="Percent">
       <calculatedColumnFormula>($P17+$Q17)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="306" totalsRowDxfId="305" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="381" totalsRowDxfId="380" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O17*$R17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="304" totalsRowDxfId="303" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="379" totalsRowDxfId="378" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R17-$S$20,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="302" totalsRowDxfId="301" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="377" totalsRowDxfId="376" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T17*$O17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="300" totalsRowDxfId="299" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="375" totalsRowDxfId="374" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U20)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -10369,20 +11367,20 @@
   <autoFilter ref="F15:L18"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="298" totalsRowDxfId="297" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="296" totalsRowDxfId="295" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="373" totalsRowDxfId="372" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="371" totalsRowDxfId="370" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G16</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="294" totalsRowDxfId="293" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="369" totalsRowDxfId="368" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$16:$H16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="292" totalsRowDxfId="291" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="367" totalsRowDxfId="366" dataCellStyle="Percent">
       <calculatedColumnFormula>$I16-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="290" totalsRowDxfId="289" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="365" totalsRowDxfId="364" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$16:$H16)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="288" totalsRowDxfId="287" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="363" totalsRowDxfId="362" dataCellStyle="Percent">
       <calculatedColumnFormula>$K16-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10394,22 +11392,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table3789" displayName="Table3789" ref="O23:V27" totalsRowCount="1">
   <autoFilter ref="O23:V26"/>
   <tableColumns count="8">
-    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="286" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="285" dataCellStyle="Currency"/>
-    <tableColumn id="4" name="CashFlow" totalsRowDxfId="284" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Ret" dataDxfId="283" totalsRowDxfId="282" dataCellStyle="Percent">
+    <tableColumn id="2" name="Probability" totalsRowLabel="Expected Value" totalsRowDxfId="361" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="YrEndPrice" totalsRowDxfId="360" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="CashFlow" totalsRowDxfId="359" dataCellStyle="Currency"/>
+    <tableColumn id="5" name="Ret" dataDxfId="358" totalsRowDxfId="357" dataCellStyle="Percent">
       <calculatedColumnFormula>($P24+$Q24)/100-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="281" totalsRowDxfId="280" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="6" name="Weighted" totalsRowFunction="sum" dataDxfId="356" totalsRowDxfId="355" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>$O24*$R24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Var" dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="1" name="Var" dataDxfId="354" totalsRowDxfId="353" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>POWER($R24-$S$27,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="277" totalsRowDxfId="276" dataCellStyle="Comma" totalsRowCellStyle="Comma">
+    <tableColumn id="7" name="WtdVar" totalsRowFunction="sum" dataDxfId="352" totalsRowDxfId="351" dataCellStyle="Comma" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>$T24*$O24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="275" totalsRowDxfId="274" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="8" name="StdDev" totalsRowFunction="custom" dataDxfId="350" totalsRowDxfId="349" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <totalsRowFormula>SQRT($U27)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -10422,20 +11420,20 @@
   <autoFilter ref="F23:L28"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Yr" totalsRowLabel="Expected"/>
-    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="273" totalsRowDxfId="272" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="GrossRet" dataDxfId="271" totalsRowDxfId="270" dataCellStyle="Percent">
+    <tableColumn id="2" name="Return" totalsRowFunction="average" dataDxfId="348" totalsRowDxfId="347" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="GrossRet" dataDxfId="346" totalsRowDxfId="345" dataCellStyle="Percent">
       <calculatedColumnFormula>1+$G24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="CumVal" dataDxfId="269" totalsRowDxfId="268" dataCellStyle="Comma">
+    <tableColumn id="4" name="CumVal" dataDxfId="344" totalsRowDxfId="343" dataCellStyle="Comma">
       <calculatedColumnFormula>PRODUCT($H$24:$H24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="HoldPerRet" dataDxfId="267" totalsRowDxfId="266" dataCellStyle="Percent">
+    <tableColumn id="5" name="HoldPerRet" dataDxfId="342" totalsRowDxfId="341" dataCellStyle="Percent">
       <calculatedColumnFormula>$I24-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="GeoMean" dataDxfId="265" totalsRowDxfId="264" dataCellStyle="Percent">
+    <tableColumn id="6" name="GeoMean" dataDxfId="340" totalsRowDxfId="339" dataCellStyle="Percent">
       <calculatedColumnFormula>GEOMEAN($H$24:$H24)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="GeoAveRet" dataDxfId="263" totalsRowDxfId="262" dataCellStyle="Percent">
+    <tableColumn id="7" name="GeoAveRet" dataDxfId="338" totalsRowDxfId="337" dataCellStyle="Percent">
       <calculatedColumnFormula>$K24-1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -12094,7 +13092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+    <sheetView topLeftCell="AF1" workbookViewId="0">
       <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
@@ -12351,12 +13349,1168 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BM20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="BO1" sqref="BO1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.6328125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.81640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6328125" style="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.6328125" style="34" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" customWidth="1"/>
+    <col min="36" max="36" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="8.7265625" style="12"/>
+    <col min="48" max="48" width="11.36328125" customWidth="1"/>
+    <col min="50" max="50" width="10.90625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="8.7265625" style="38"/>
+    <col min="52" max="52" width="10.6328125" style="2" customWidth="1"/>
+    <col min="53" max="53" width="9.81640625" customWidth="1"/>
+    <col min="54" max="55" width="8.7265625" style="2"/>
+    <col min="56" max="56" width="10.36328125" customWidth="1"/>
+    <col min="58" max="58" width="11.36328125" style="34" customWidth="1"/>
+    <col min="60" max="60" width="11.36328125" customWidth="1"/>
+    <col min="61" max="61" width="13.36328125" style="2" customWidth="1"/>
+    <col min="62" max="62" width="8.7265625" style="2"/>
+    <col min="64" max="64" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="R1" t="s">
+        <v>185</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT1" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY1" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BB1"/>
+      <c r="BC1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>202</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>160</v>
+      </c>
+      <c r="BF1" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>183</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="E2" s="6">
+        <f>B2-A2</f>
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="F2" s="34">
+        <f>C2*C2</f>
+        <v>4.2024999999999993E-2</v>
+      </c>
+      <c r="G2" s="34">
+        <f>E2/(D2*F2)</f>
+        <v>2.9652679266004673</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="K2" s="34">
+        <v>1.21E-2</v>
+      </c>
+      <c r="L2" s="34">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="M2" s="34">
+        <v>0.45</v>
+      </c>
+      <c r="N2" s="2">
+        <f>SQRT(K2)</f>
+        <v>0.11</v>
+      </c>
+      <c r="O2" s="2">
+        <f>SQRT(L2)</f>
+        <v>0.13</v>
+      </c>
+      <c r="P2" s="2">
+        <f>J2-I2</f>
+        <v>0.06</v>
+      </c>
+      <c r="Q2" s="34">
+        <f>M2*O2/N2</f>
+        <v>0.53181818181818186</v>
+      </c>
+      <c r="R2" s="15">
+        <f>I2+Q2*P2</f>
+        <v>5.1909090909090905E-2</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="X2" s="2">
+        <f>U2-T2</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y2" s="2">
+        <f>W2-T2</f>
+        <v>0.09</v>
+      </c>
+      <c r="Z2" s="2">
+        <f>V2*Y2/X2</f>
+        <v>0.2314285714285714</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="AF2" s="2">
+        <f>AC2-AB2</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AG2" s="2">
+        <f>AF2*AE2/AD2</f>
+        <v>0.15555555555555559</v>
+      </c>
+      <c r="AH2" s="2">
+        <f>AG2+AB2</f>
+        <v>0.18555555555555558</v>
+      </c>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="AL2" s="2">
+        <f>AK2-AJ2</f>
+        <v>0.06</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>5000</v>
+      </c>
+      <c r="AP2">
+        <v>0.75</v>
+      </c>
+      <c r="AQ2">
+        <f t="shared" ref="AQ2:AQ5" si="0">AO2/AO$6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="AR2">
+        <f t="shared" ref="AR2:AR5" si="1">AP2*AQ2</f>
+        <v>0.125</v>
+      </c>
+      <c r="AS2" s="12">
+        <f t="shared" ref="AS2:AS5" si="2">$AJ$2+AP2*$AL$2</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AT2" s="12">
+        <f t="shared" ref="AT2:AT5" si="3">AQ2*AS2</f>
+        <v>1.0833333333333334E-2</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW2">
+        <v>0.1</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AY2" s="38">
+        <f t="shared" ref="AY2:AY4" si="4">AX2/50-1</f>
+        <v>-0.19999999999999996</v>
+      </c>
+      <c r="AZ2" s="2">
+        <f t="shared" ref="AZ2:AZ4" si="5">AW2*AY2</f>
+        <v>-1.9999999999999997E-2</v>
+      </c>
+      <c r="BA2">
+        <f t="shared" ref="BA2:BA4" si="6">AW2*POWER(AY2-AZ$5,2)</f>
+        <v>7.8400000000000015E-3</v>
+      </c>
+      <c r="BB2"/>
+      <c r="BC2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BD2" s="6">
+        <f>BA6</f>
+        <v>9.7979589711327114E-2</v>
+      </c>
+      <c r="BE2">
+        <v>0.8</v>
+      </c>
+      <c r="BF2" s="34">
+        <f>BE2*BD2/BC2</f>
+        <v>0.78383671769061691</v>
+      </c>
+      <c r="BH2">
+        <v>0.8</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="BJ2" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="BK2" s="6">
+        <f>BJ2-BI2</f>
+        <v>0.06</v>
+      </c>
+      <c r="BL2" s="2">
+        <f>BH2*BK2</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="BM2" s="2">
+        <f>BL2+BI2</f>
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AN3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AP3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AQ3">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AR3">
+        <f t="shared" si="1"/>
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="AS3" s="12">
+        <f t="shared" si="2"/>
+        <v>8.6000000000000007E-2</v>
+      </c>
+      <c r="AT3" s="12">
+        <f t="shared" si="3"/>
+        <v>2.8666666666666667E-2</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW3">
+        <v>0.8</v>
+      </c>
+      <c r="AX3" s="1">
+        <v>55</v>
+      </c>
+      <c r="AY3" s="38">
+        <f t="shared" si="4"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AZ3" s="2">
+        <f t="shared" si="5"/>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="BA3">
+        <f t="shared" si="6"/>
+        <v>3.2000000000000062E-4</v>
+      </c>
+      <c r="BB3"/>
+      <c r="BC3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BD3" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="BE3">
+        <v>0.54</v>
+      </c>
+      <c r="BF3" s="34">
+        <f>BE3*BD3/BC3</f>
+        <v>0.64799999999999991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AN4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>8000</v>
+      </c>
+      <c r="AP4">
+        <v>1.36</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="AR4">
+        <f t="shared" si="1"/>
+        <v>0.36266666666666669</v>
+      </c>
+      <c r="AS4" s="12">
+        <f t="shared" si="2"/>
+        <v>0.10160000000000001</v>
+      </c>
+      <c r="AT4" s="12">
+        <f t="shared" si="3"/>
+        <v>2.7093333333333334E-2</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW4">
+        <v>0.1</v>
+      </c>
+      <c r="AX4" s="1">
+        <v>60</v>
+      </c>
+      <c r="AY4" s="38">
+        <f t="shared" si="4"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AZ4" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+      <c r="BA4">
+        <f t="shared" si="6"/>
+        <v>1.4399999999999973E-3</v>
+      </c>
+      <c r="BB4"/>
+      <c r="BC4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BD4" s="6">
+        <v>5.2201532544552724E-2</v>
+      </c>
+      <c r="BE4">
+        <v>0.9</v>
+      </c>
+      <c r="BF4" s="34">
+        <f>BE4*BD4/BC4</f>
+        <v>0.46981379290097447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AN5" t="s">
+        <v>191</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>7000</v>
+      </c>
+      <c r="AP5">
+        <v>1.88</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="AR5">
+        <f t="shared" si="1"/>
+        <v>0.43866666666666665</v>
+      </c>
+      <c r="AS5" s="12">
+        <f t="shared" si="2"/>
+        <v>0.13279999999999997</v>
+      </c>
+      <c r="AT5" s="12">
+        <f t="shared" si="3"/>
+        <v>3.0986666666666662E-2</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AW5">
+        <f>SUBTOTAL(109,Table43[Prob])</f>
+        <v>1</v>
+      </c>
+      <c r="AX5" s="14"/>
+      <c r="AZ5" s="11">
+        <f>SUBTOTAL(109,Table43[RetWtdAve])</f>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="BA5">
+        <f>SUBTOTAL(109,Table43[VarSub])</f>
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="BB5"/>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AN6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO6" s="39">
+        <f>SUBTOTAL(109,Table41[Invested])</f>
+        <v>30000</v>
+      </c>
+      <c r="AQ6">
+        <f>SUBTOTAL(109,Table41[Weight])</f>
+        <v>1</v>
+      </c>
+      <c r="AR6">
+        <f>SUBTOTAL(109,Table41[BetaWtdAve])</f>
+        <v>1.2930000000000001</v>
+      </c>
+      <c r="AT6" s="12">
+        <f>SUBTOTAL(109,Table41[RetWtdAve])</f>
+        <v>9.758E-2</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA6" s="2">
+        <f>SQRT(BA5)</f>
+        <v>9.7979589711327114E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV8" t="s">
+        <v>197</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AX8" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY8" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV9" t="s">
+        <v>216</v>
+      </c>
+      <c r="AW9">
+        <v>0.3</v>
+      </c>
+      <c r="AX9" s="1">
+        <v>55</v>
+      </c>
+      <c r="AY9" s="38">
+        <f t="shared" ref="AY9:AY11" si="7">AX9/50-1</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AZ9" s="2">
+        <f t="shared" ref="AZ9:AZ11" si="8">AW9*AY9</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="BA9">
+        <f t="shared" ref="BA9:BA11" si="9">AW9*POWER(AY9-AZ$12,2)</f>
+        <v>9.0749999999999598E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW10">
+        <v>0.5</v>
+      </c>
+      <c r="AX10" s="1">
+        <v>57.5</v>
+      </c>
+      <c r="AY10" s="38">
+        <f t="shared" si="7"/>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="AZ10" s="2">
+        <f t="shared" si="8"/>
+        <v>7.4999999999999956E-2</v>
+      </c>
+      <c r="BA10">
+        <f t="shared" si="9"/>
+        <v>1.25000000000003E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW11">
+        <v>0.2</v>
+      </c>
+      <c r="AX11" s="1">
+        <v>62.5</v>
+      </c>
+      <c r="AY11" s="38">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+      <c r="AZ11" s="2">
+        <f t="shared" si="8"/>
+        <v>0.05</v>
+      </c>
+      <c r="BA11">
+        <f t="shared" si="9"/>
+        <v>1.805000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV12" t="s">
+        <v>20</v>
+      </c>
+      <c r="AW12">
+        <f>SUBTOTAL(109,Table4348[Prob])</f>
+        <v>1</v>
+      </c>
+      <c r="AX12" s="14"/>
+      <c r="AZ12" s="11">
+        <f>SUBTOTAL(109,Table4348[RetWtdAve])</f>
+        <v>0.15499999999999997</v>
+      </c>
+      <c r="BA12">
+        <f>SUBTOTAL(109,Table4348[VarSub])</f>
+        <v>2.7249999999999974E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV13" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA13" s="2">
+        <f>SQRT(BA12)</f>
+        <v>5.2201532544552724E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV15" t="s">
+        <v>197</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AX15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY15" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AZ15" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="AV16" t="s">
+        <v>216</v>
+      </c>
+      <c r="AW16">
+        <v>0.3</v>
+      </c>
+      <c r="AX16" s="1">
+        <v>47.5</v>
+      </c>
+      <c r="AY16" s="38">
+        <f t="shared" ref="AY16:AY18" si="10">AX16/50-1</f>
+        <v>-5.0000000000000044E-2</v>
+      </c>
+      <c r="AZ16" s="2">
+        <f t="shared" ref="AZ16:AZ18" si="11">AW16*AY16</f>
+        <v>-1.5000000000000013E-2</v>
+      </c>
+      <c r="BA16">
+        <f t="shared" ref="BA16:BA18" si="12">AW16*POWER(AY16-AZ$12,2)</f>
+        <v>1.2607500000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="48:53" x14ac:dyDescent="0.3">
+      <c r="AV17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW17">
+        <v>0.5</v>
+      </c>
+      <c r="AX17" s="1">
+        <v>60</v>
+      </c>
+      <c r="AY17" s="38">
+        <f t="shared" si="10"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AZ17" s="2">
+        <f t="shared" si="11"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="BA17">
+        <f t="shared" si="12"/>
+        <v>1.0124999999999993E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="48:53" x14ac:dyDescent="0.3">
+      <c r="AV18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW18">
+        <v>0.2</v>
+      </c>
+      <c r="AX18" s="1">
+        <v>65</v>
+      </c>
+      <c r="AY18" s="38">
+        <f t="shared" si="10"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AZ18" s="2">
+        <f t="shared" si="11"/>
+        <v>6.0000000000000012E-2</v>
+      </c>
+      <c r="BA18">
+        <f t="shared" si="12"/>
+        <v>4.2050000000000047E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="48:53" x14ac:dyDescent="0.3">
+      <c r="AV19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AW19">
+        <f>SUBTOTAL(109,Table434849[Prob])</f>
+        <v>1</v>
+      </c>
+      <c r="AX19" s="14"/>
+      <c r="AZ19" s="11">
+        <f>SUBTOTAL(109,Table434849[RetWtdAve])</f>
+        <v>0.14499999999999996</v>
+      </c>
+      <c r="BA19">
+        <f>SUBTOTAL(109,Table434849[VarSub])</f>
+        <v>1.7825000000000008E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="48:53" x14ac:dyDescent="0.3">
+      <c r="AV20" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA20" s="2">
+        <f>SQRT(BA19)</f>
+        <v>0.13351029922818691</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="11">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="6" width="8.7265625" style="2"/>
+    <col min="8" max="8" width="12.36328125" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.215</v>
+      </c>
+      <c r="B2">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5.3E-3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H2" s="6">
+        <f>G2+SUMPRODUCT(A2:C2,D2:F2)</f>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="I2" s="15">
+        <f>12*H2</f>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:W8"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="22" max="22" width="10.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" t="s">
+        <v>163</v>
+      </c>
+      <c r="M2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>222</v>
+      </c>
+      <c r="R2" t="s">
+        <v>223</v>
+      </c>
+      <c r="S2" t="s">
+        <v>224</v>
+      </c>
+      <c r="T2" t="s">
+        <v>225</v>
+      </c>
+      <c r="U2" t="s">
+        <v>226</v>
+      </c>
+      <c r="V2" t="s">
+        <v>227</v>
+      </c>
+      <c r="W2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3">
+        <v>2.7249999999999974E-3</v>
+      </c>
+      <c r="F3">
+        <v>2.8710842899503999E-3</v>
+      </c>
+      <c r="H3">
+        <f t="array" ref="H3:I3">MMULT(A3:B3,E3:F4)</f>
+        <v>2.7980421449751987E-3</v>
+      </c>
+      <c r="I3">
+        <v>7.4855421449751998E-3</v>
+      </c>
+      <c r="K3">
+        <f t="array" ref="K3:K4">TRANSPOSE(A3:B3)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M3">
+        <f>MMULT(H3:I3,K3:K4)</f>
+        <v>5.1417921449751994E-3</v>
+      </c>
+      <c r="N3">
+        <f>SQRT(M3)</f>
+        <v>7.1706290832640338E-2</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
+      <c r="Q3">
+        <v>0.9</v>
+      </c>
+      <c r="R3">
+        <v>0.26</v>
+      </c>
+      <c r="S3">
+        <f>Q3*$P3*A6</f>
+        <v>4.6981379290097457E-3</v>
+      </c>
+      <c r="T3">
+        <f>R3*$P3*B6</f>
+        <v>2.8600000000000001E-3</v>
+      </c>
+      <c r="U3">
+        <f>SUMPRODUCT(A3:B3,S3:T3)</f>
+        <v>3.7790689645048727E-3</v>
+      </c>
+      <c r="V3">
+        <f>U3/(P3*N3)</f>
+        <v>0.52702056132356234</v>
+      </c>
+      <c r="W3">
+        <f>V3*N3/P3</f>
+        <v>0.37790689645048725</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4">
+        <v>2.8710842899503999E-3</v>
+      </c>
+      <c r="F4">
+        <v>1.21E-2</v>
+      </c>
+      <c r="K4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5.2201532544552724E-2</v>
+      </c>
+      <c r="B6">
+        <v>0.11</v>
+      </c>
+      <c r="E6">
+        <f>A6*A6</f>
+        <v>2.7249999999999974E-3</v>
+      </c>
+      <c r="F6">
+        <f>B6*B6</f>
+        <v>1.21E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8">
+        <f>E7*A6*B6</f>
+        <v>2.8710842899503999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW22"/>
   <sheetViews>
-    <sheetView topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BY1" sqref="BY1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>